<commit_message>
fixed google review bug
</commit_message>
<xml_diff>
--- a/raw-apartments.xlsx
+++ b/raw-apartments.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V63"/>
+  <dimension ref="A1:V64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,16 +582,16 @@
           <t>B2</t>
         </is>
       </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="b">
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
         <v>1</v>
       </c>
       <c r="N2" t="inlineStr">
@@ -599,25 +599,25 @@
           <t>4.6</t>
         </is>
       </c>
-      <c r="O2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U2" t="b">
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
         <v>1</v>
       </c>
       <c r="V2" t="inlineStr">
@@ -890,40 +890,40 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>IMT Lakeshore Lofts</t>
+          <t>Cortland MacArthur</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/imt-lakeshore-lofts-irving-tx/wpg4b6l/</t>
+          <t>https://www.apartments.com/cortland-macarthur-irving-tx/k9n8jj9/</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>800 Lake Carolyn Pky, Irving, TX 75039</t>
+          <t>7904 N Glen Dr, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Urban Center Irving</t>
+          <t>Valley Ranch</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2,225</t>
+          <t>2,169</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1,169</t>
+          <t>1,069</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>1.903336184773311</v>
+        <v>2.028999064546305</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>The Lucca</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -940,7 +940,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="O6" t="b">
@@ -966,7 +966,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $2,225 – $2,275, 2 beds, 2 baths, 1,169 sq ft, Available Now, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Dining Room, Recreation Room, Views, Walk-In Closets, Window Coverings, Large Bedrooms, </t>
+          <t xml:space="preserve">The Lucca, $2,169 – $2,179, 2 beds, 2 baths, 1,069 sq ft, Tour This Floor Plan, View The Lucca, Floor Plan, View The Lucca Floor Plan Details, Show Floor Plan Details, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 773101, price, $2,179, square feet, 1,069, availibility, Now, Unit 773101, Unit, 713062, price, $2,179, square feet, 1,069, availibility, Mar. 24, Unit 713062, Unit, 453021, price, $2,179, square feet, 1,069, availibility, Apr. 8, Unit 453021, </t>
         </is>
       </c>
     </row>
@@ -976,40 +976,40 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AVE Las Colinas</t>
+          <t>IMT Lakeshore Lofts</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/ave-las-colinas-irving-tx/qfsptny/</t>
+          <t>https://www.apartments.com/imt-lakeshore-lofts-irving-tx/wpg4b6l/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1501 Meridian Dr, Irving, TX 75039</t>
+          <t>800 Lake Carolyn Pky, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Urban Center Irving</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2,435</t>
+          <t>2,225</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1,161</t>
+          <t>1,169</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2.097329888027562</v>
+        <v>1.903336184773311</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>B2G</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="O7" t="b">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2G, $2,435, 2 beds, 2 baths, 1,161 sq ft, Tour This Floor Plan, View B2G, Floor Plan, View B2G Floor Plan Details, Hide Floor Plan Details, Highlights, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Views, Walk-In Closets, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 2202, price, $2,435, square feet, 1,161, availibility, Apr. 13, Unit 2202, </t>
+          <t xml:space="preserve">B1, $2,225 – $2,275, 2 beds, 2 baths, 1,169 sq ft, Available Now, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Dining Room, Recreation Room, Views, Walk-In Closets, Window Coverings, Large Bedrooms, </t>
         </is>
       </c>
     </row>
@@ -1062,17 +1062,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cortland La Villita</t>
+          <t>AVE Las Colinas</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/cortland-la-villita-irving-tx/cmvjm0f/</t>
+          <t>https://www.apartments.com/ave-las-colinas-irving-tx/qfsptny/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6419 Tranquilo, Irving, TX 75039</t>
+          <t>1501 Meridian Dr, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1082,20 +1082,20 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2,307</t>
+          <t>2,435</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1,156</t>
+          <t>1,161</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>1.995674740484429</v>
+        <v>2.097329888027562</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Terracotta</t>
+          <t>B2G</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="O8" t="b">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Terracotta, $2,307 – $2,332, 2 beds, 2 baths, 1,156 sq ft, Tour This Floor Plan, View Terracotta, Floor Plan, View Terracotta Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Storage Units, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Eat-in Kitchen, Kitchen, Microwave, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Yard, Lawn, Hardwood Floors, Tile Floors, Vinyl Flooring, Dining Room, Crown Molding, Vaulted Ceiling, Views, Walk-In Closets, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 2015, price, $2,332, square feet, 1,156, availibility, Now, Unit 2015, Unit, 3026, price, $2,307, square feet, 1,156, availibility, Mar. 26, Unit 3026, Unit, 3010, price, $2,317, square feet, 1,156, availibility, Apr. 26, Unit 3010, </t>
+          <t xml:space="preserve">B2G, $2,435, 2 beds, 2 baths, 1,161 sq ft, Tour This Floor Plan, View B2G, Floor Plan, View B2G Floor Plan Details, Hide Floor Plan Details, Highlights, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Views, Walk-In Closets, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 2202, price, $2,435, square feet, 1,161, availibility, Apr. 13, Unit 2202, </t>
         </is>
       </c>
     </row>
@@ -1148,40 +1148,40 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>AMLI Las Colinas</t>
+          <t>Cortland La Villita</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/amli-las-colinas-irving-tx/4zdbz1j/</t>
+          <t>https://www.apartments.com/cortland-la-villita-irving-tx/cmvjm0f/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1050 Lake Carolyn Pky, Irving, TX 75039</t>
+          <t>6419 Tranquilo, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Urban Center Irving</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2,097</t>
+          <t>2,307</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1,252</t>
+          <t>1,156</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1.674920127795527</v>
+        <v>1.995674740484429</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>C650</t>
+          <t>Terracotta</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="O9" t="b">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t xml:space="preserve">C650, $2,097 – $2,937, 2 beds, 2 baths, 1,252 sq ft, $500 deposit, Available Now, Tour This Floor Plan, View C650, Floor Plan, View C650, Virtual Tours, View C650 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Double Vanities, Tub/Shower, Fireplace, Surround Sound, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Dining Room, Family Room, Mud Room, Office, Den, Vaulted Ceiling, Views, Walk-In Closets, Loft Layout, Window Coverings, Large Bedrooms, </t>
+          <t xml:space="preserve">Terracotta, $2,307 – $2,332, 2 beds, 2 baths, 1,156 sq ft, Tour This Floor Plan, View Terracotta, Floor Plan, View Terracotta Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Storage Units, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Eat-in Kitchen, Kitchen, Microwave, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Yard, Lawn, Hardwood Floors, Tile Floors, Vinyl Flooring, Dining Room, Crown Molding, Vaulted Ceiling, Views, Walk-In Closets, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 2015, price, $2,332, square feet, 1,156, availibility, Now, Unit 2015, Unit, 3026, price, $2,307, square feet, 1,156, availibility, Mar. 26, Unit 3026, Unit, 3010, price, $2,317, square feet, 1,156, availibility, Apr. 26, Unit 3010, </t>
         </is>
       </c>
     </row>
@@ -1234,40 +1234,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fountain Pointe Las Colinas</t>
+          <t>AMLI Las Colinas</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/fountain-pointe-las-colinas-irving-tx/kzm4m29/</t>
+          <t>https://www.apartments.com/amli-las-colinas-irving-tx/4zdbz1j/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5225 W Las Colinas Blvd, Irving, TX 75039</t>
+          <t>1050 Lake Carolyn Pky, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Urban Center Irving</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2,057</t>
+          <t>2,097</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1,221</t>
+          <t>1,252</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1.684684684684685</v>
+        <v>1.674920127795527</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2 Bed 2 Bath</t>
+          <t>C650</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -1284,7 +1284,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="O10" t="b">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 Bed 2 Bath, $2,057 – $3,795, 2 beds, 2 baths, 1,221 sq ft, Tour This Floor Plan, View 2 Bed 2 Bath, Floor Plan, View 2 Bed 2 Bath Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Double Vanities, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Breakfast Nook, Floor Plan Details, Balcony, Patio, Yard, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 4045, price, $2,087, square feet, 1,003, availibility, Now, Unit 4045, Unit, 4101, price, $2,276, square feet, 1,221, availibility, Mar. 19, Unit 4101, Unit, 2085, price, $2,276, square feet, 1,221, availibility, Mar. 21, Unit 2085, </t>
+          <t xml:space="preserve">C650, $2,097 – $2,937, 2 beds, 2 baths, 1,252 sq ft, $500 deposit, Available Now, Tour This Floor Plan, View C650, Floor Plan, View C650, Virtual Tours, View C650 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Double Vanities, Tub/Shower, Fireplace, Surround Sound, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Dining Room, Family Room, Mud Room, Office, Den, Vaulted Ceiling, Views, Walk-In Closets, Loft Layout, Window Coverings, Large Bedrooms, </t>
         </is>
       </c>
     </row>
@@ -1320,17 +1320,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AMLI on Riverside</t>
+          <t>Fountain Pointe Las Colinas</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/amli-on-riverside-irving-tx/9kg0qp6/</t>
+          <t>https://www.apartments.com/fountain-pointe-las-colinas-irving-tx/kzm4m29/</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>310 Gran Via, Irving, TX 75039</t>
+          <t>5225 W Las Colinas Blvd, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2,133</t>
+          <t>2,057</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1349,11 +1349,11 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>1.746928746928747</v>
+        <v>1.684684684684685</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>C6a</t>
+          <t>2 Bed 2 Bath</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="O11" t="b">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t xml:space="preserve">C6a, $2,133 – $2,625, 2 beds, 2 baths, 1,221 sq ft, $500 deposit, Apr. 26, Tour This Floor Plan, View C6a, Floor Plan, View C6a Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Lawn, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Office, Den, Views, Walk-In Closets, Double Pane Windows, Window Coverings, Large Bedrooms, </t>
+          <t xml:space="preserve">2 Bed 2 Bath, $2,057 – $3,795, 2 beds, 2 baths, 1,221 sq ft, Tour This Floor Plan, View 2 Bed 2 Bath, Floor Plan, View 2 Bed 2 Bath Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Double Vanities, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Breakfast Nook, Floor Plan Details, Balcony, Patio, Yard, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 4045, price, $2,087, square feet, 1,003, availibility, Now, Unit 4045, Unit, 4101, price, $2,276, square feet, 1,221, availibility, Mar. 19, Unit 4101, Unit, 2085, price, $2,276, square feet, 1,221, availibility, Mar. 21, Unit 2085, </t>
         </is>
       </c>
     </row>
@@ -1406,17 +1406,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>La Villita Lakeside and Landings</t>
+          <t>AMLI on Riverside</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/la-villita-lakeside-and-landings-irving-tx/7cc8s3x/</t>
+          <t>https://www.apartments.com/amli-on-riverside-irving-tx/9kg0qp6/</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6727 Deseo, Irving, TX 75039</t>
+          <t>310 Gran Via, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1426,20 +1426,20 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2,645</t>
+          <t>2,133</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1,168</t>
+          <t>1,221</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>2.264554794520548</v>
+        <v>1.746928746928747</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>B3-LL GARAGE</t>
+          <t>C6a</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="O12" t="b">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t xml:space="preserve">B3-LL GARAGE, $2,645 – $3,848, 2 beds, 2 baths, 1,168 sq ft, $200 deposit, Available Now, Tour This Floor Plan, View B3-LL GARAGE, Floor Plan, View B3-LL GARAGE Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Tub/Shower, Fireplace, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Office, Sunroom, Crown Molding, Vaulted Ceiling, Views, Walk-In Closets, Double Pane Windows, Window Coverings, Large Bedrooms, </t>
+          <t xml:space="preserve">C6a, $2,133 – $2,625, 2 beds, 2 baths, 1,221 sq ft, $500 deposit, Apr. 26, Tour This Floor Plan, View C6a, Floor Plan, View C6a Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Lawn, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Office, Den, Views, Walk-In Closets, Double Pane Windows, Window Coverings, Large Bedrooms, </t>
         </is>
       </c>
     </row>
@@ -1492,40 +1492,40 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Mercer 1900</t>
+          <t>La Villita Lakeside and Landings</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/mercer-1900-farmers-branch-tx/wgr52vh/</t>
+          <t>https://www.apartments.com/la-villita-lakeside-and-landings-irving-tx/7cc8s3x/</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1900 Knightsbridge Rd, Farmers Branch, TX 75234</t>
+          <t>6727 Deseo, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Koreatown/Gribble</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2,130</t>
+          <t>2,645</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1,152</t>
+          <t>1,168</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>1.848958333333333</v>
+        <v>2.264554794520548</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B3-LL GARAGE</t>
         </is>
       </c>
       <c r="J13" t="b">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="O13" t="b">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t xml:space="preserve">B3, $2,130 – $3,289, 2 beds, 2 baths, 1,152 sq ft, Tour This Floor Plan, View B3, Floor Plan, View B3 Floor Plan Details, Hide Floor Plan Details, Highlights, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Walk-In Closets, Double Pane Windows, Window Coverings, 5 Available units, Unit, Price, Sq Ft, Availability, Unit, 3-3324, price, $2,130, square feet, 1,152, availibility, Now, Unit 3-3324, Unit, 5-5308, price, $2,140, square feet, 1,152, availibility, Now, Unit 5-5308, Unit, 6-6104, price, $2,195, square feet, 1,152, availibility, Now, Unit 6-6104, Show More Results (2), </t>
+          <t xml:space="preserve">B3-LL GARAGE, $2,645 – $3,848, 2 beds, 2 baths, 1,168 sq ft, $200 deposit, Available Now, Tour This Floor Plan, View B3-LL GARAGE, Floor Plan, View B3-LL GARAGE Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Tub/Shower, Fireplace, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Office, Sunroom, Crown Molding, Vaulted Ceiling, Views, Walk-In Closets, Double Pane Windows, Window Coverings, Large Bedrooms, </t>
         </is>
       </c>
     </row>
@@ -1578,40 +1578,40 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Aspen at Mercer Crossing</t>
+          <t>Mercer 1900</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/aspen-at-mercer-crossing-farmers-branch-tx/mmet0zj/</t>
+          <t>https://www.apartments.com/mercer-1900-farmers-branch-tx/wgr52vh/</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1851 Knightsbridge Rd, Farmers Branch, TX 75234</t>
+          <t>1900 Knightsbridge Rd, Farmers Branch, TX 75234</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Farmers Branch</t>
+          <t>Koreatown/Gribble</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2,160</t>
+          <t>2,130</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1,337</t>
+          <t>1,152</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>1.615557217651459</v>
+        <v>1.848958333333333</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2D</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="J14" t="b">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="O14" t="b">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t xml:space="preserve">2D, $2,160 – $3,565, 2 beds, 2 baths, 1,337 sq ft, $200 deposit, Tour This Floor Plan, View 2D, Floor Plan, View 2D, Virtual Tours, View 2D Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Trash Compactor, Storage Units, Tub/Shower, Sprinkler System, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Built-In Bookshelves, Crown Molding, Vaulted Ceiling, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 3302, price, $2,160, square feet, 1,337, availibility, Apr. 1, Unit 3302, </t>
+          <t xml:space="preserve">B3, $2,130 – $3,289, 2 beds, 2 baths, 1,152 sq ft, Tour This Floor Plan, View B3, Floor Plan, View B3 Floor Plan Details, Hide Floor Plan Details, Highlights, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Walk-In Closets, Double Pane Windows, Window Coverings, 5 Available units, Unit, Price, Sq Ft, Availability, Unit, 3-3324, price, $2,130, square feet, 1,152, availibility, Now, Unit 3-3324, Unit, 5-5308, price, $2,140, square feet, 1,152, availibility, Now, Unit 5-5308, Unit, 6-6104, price, $2,195, square feet, 1,152, availibility, Now, Unit 6-6104, Show More Results (2), </t>
         </is>
       </c>
     </row>
@@ -1664,47 +1664,47 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Avenue 900</t>
+          <t>Aspen at Mercer Crossing</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/avenue-900-euless-tx/5380x4q/</t>
+          <t>https://www.apartments.com/aspen-at-mercer-crossing-farmers-branch-tx/mmet0zj/</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>900 Grange Hall Dr, Euless, TX 76039</t>
+          <t>1851 Knightsbridge Rd, Farmers Branch, TX 75234</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Hurst/Euless/Bedford</t>
+          <t>Farmers Branch</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>1,985</t>
+          <t>2,160</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1,119</t>
+          <t>1,337</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>1.77390527256479</v>
+        <v>1.615557217651459</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>2D</t>
         </is>
       </c>
       <c r="J15" t="b">
         <v>1</v>
       </c>
       <c r="K15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="b">
         <v>1</v>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="O15" t="b">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2, $1,985 – $2,171, 2 beds, 2 baths, 1,119 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Tub/Shower, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Dining Room, Walk-In Closets, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 5214, price, $1,985, square feet, 1,119, availibility, Now, Unit 5214, Unit, 7324, price, $2,020, square feet, 1,119, availibility, Now, Unit 7324, </t>
+          <t xml:space="preserve">2D, $2,160 – $3,565, 2 beds, 2 baths, 1,337 sq ft, $200 deposit, Tour This Floor Plan, View 2D, Floor Plan, View 2D, Virtual Tours, View 2D Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Trash Compactor, Storage Units, Tub/Shower, Sprinkler System, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Built-In Bookshelves, Crown Molding, Vaulted Ceiling, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 3302, price, $2,160, square feet, 1,337, availibility, Apr. 1, Unit 3302, </t>
         </is>
       </c>
     </row>
@@ -1750,47 +1750,47 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sage Hill at Cypress Waters</t>
+          <t>Avenue 900</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/sage-hill-at-cypress-waters-coppell-tx/kew4zv8/</t>
+          <t>https://www.apartments.com/avenue-900-euless-tx/5380x4q/</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2275 Sage Hill Ln, Coppell, TX 75019</t>
+          <t>900 Grange Hall Dr, Euless, TX 76039</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Coppell</t>
+          <t>Hurst/Euless/Bedford</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2,528</t>
+          <t>1,985</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1,070</t>
+          <t>1,119</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>2.362616822429906</v>
+        <v>1.77390527256479</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2 Bedroom, 2 Bath</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="J16" t="b">
         <v>1</v>
       </c>
       <c r="K16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" t="b">
         <v>1</v>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 Bedroom, 2 Bath, $2,528 – $9,466, 2 beds, 2 baths, 1,070 sq ft, Tour This Floor Plan, View 2 Bedroom, 2 Bath, Floor Plan, View 2 Bedroom, 2 Bath Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Mud Room, Office, Recreation Room, Den, Built-In Bookshelves, Vaulted Ceiling, Walk-In Closets, Linen Closet, Window Coverings, 27 Available units, Unit, Price, Sq Ft, Availability, Unit, 17-17202, price, $2,528, square feet, 1,148, availibility, Now, Unit 17-17202, Unit, 19-19207, price, $2,543, square feet, 1,229, availibility, Now, Unit 19-19207, Unit, 03-3311, price, $2,587, square feet, 1,258, availibility, Now, Unit 03-3311, Show More Results (24), </t>
+          <t xml:space="preserve">B2, $1,985 – $2,171, 2 beds, 2 baths, 1,119 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Tub/Shower, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Dining Room, Walk-In Closets, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 5214, price, $1,985, square feet, 1,119, availibility, Now, Unit 5214, Unit, 7324, price, $2,020, square feet, 1,119, availibility, Now, Unit 7324, </t>
         </is>
       </c>
     </row>
@@ -1836,40 +1836,40 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MAA Bella Casita</t>
+          <t>Sage Hill at Cypress Waters</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/maa-bella-casita-irving-tx/bw1lm1c/</t>
+          <t>https://www.apartments.com/sage-hill-at-cypress-waters-coppell-tx/kew4zv8/</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>851 Lake Carolyn Pky, Irving, TX 75039</t>
+          <t>2275 Sage Hill Ln, Coppell, TX 75019</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Urban Center Irving</t>
+          <t>Coppell</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2,353</t>
+          <t>2,528</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1,600</t>
+          <t>1,070</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>1.470625</v>
+        <v>2.362616822429906</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Acacia</t>
+          <t>2 Bedroom, 2 Bath</t>
         </is>
       </c>
       <c r="J17" t="b">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="O17" t="b">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Acacia, $2,353 – $4,193, 2 beds, 2 baths, 1,600 sq ft, Tour This Floor Plan, View Acacia, Floor Plan, View Acacia Floor Plan Details, Hide Floor Plan Details, Highlights, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Double Vanities, Sprinkler System, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Island Kitchen, Kitchen, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Den, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 01431, price, $2,353, square feet, 1,600, availibility, Mar. 11, Unit 01431, </t>
+          <t xml:space="preserve">2 Bedroom, 2 Bath, $2,528 – $9,466, 2 beds, 2 baths, 1,070 sq ft, Tour This Floor Plan, View 2 Bedroom, 2 Bath, Floor Plan, View 2 Bedroom, 2 Bath Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Mud Room, Office, Recreation Room, Den, Built-In Bookshelves, Vaulted Ceiling, Walk-In Closets, Linen Closet, Window Coverings, 27 Available units, Unit, Price, Sq Ft, Availability, Unit, 17-17202, price, $2,528, square feet, 1,148, availibility, Now, Unit 17-17202, Unit, 19-19207, price, $2,543, square feet, 1,229, availibility, Now, Unit 19-19207, Unit, 03-3311, price, $2,587, square feet, 1,258, availibility, Now, Unit 03-3311, Show More Results (24), </t>
         </is>
       </c>
     </row>
@@ -1922,17 +1922,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lakeside Urban Center</t>
+          <t>MAA Bella Casita</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/lakeside-urban-center-irving-tx/kjt6jb9/</t>
+          <t>https://www.apartments.com/maa-bella-casita-irving-tx/bw1lm1c/</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>850 Lake Carolyn Pky, Irving, TX 75039</t>
+          <t>851 Lake Carolyn Pky, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1942,20 +1942,20 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2,126</t>
+          <t>2,353</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>1,324</t>
+          <t>1,600</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>1.605740181268882</v>
+        <v>1.470625</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>B2A</t>
+          <t>Acacia</t>
         </is>
       </c>
       <c r="J18" t="b">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="O18" t="b">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2A, $2,126, 2 beds, 2 baths, 1,324 sq ft, Tour This Floor Plan, View B2A, Floor Plan, View B2A Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Views, Walk-In Closets, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 2109, price, $2,126, square feet, 1,324, availibility, Now, Unit 2109, </t>
+          <t xml:space="preserve">Acacia, $2,353 – $4,193, 2 beds, 2 baths, 1,600 sq ft, Tour This Floor Plan, View Acacia, Floor Plan, View Acacia Floor Plan Details, Hide Floor Plan Details, Highlights, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Double Vanities, Sprinkler System, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Island Kitchen, Kitchen, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Den, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 01431, price, $2,353, square feet, 1,600, availibility, Mar. 11, Unit 01431, </t>
         </is>
       </c>
     </row>
@@ -2008,40 +2008,40 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Via Las Colinas</t>
+          <t>Lakeside Urban Center</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/via-las-colinas-irving-tx/m4vqwbj/</t>
+          <t>https://www.apartments.com/lakeside-urban-center-irving-tx/kjt6jb9/</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>401 W Northwest Hwy, Irving, TX 75039</t>
+          <t>850 Lake Carolyn Pky, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Urban Center Irving</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2,213</t>
+          <t>2,126</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>1,088</t>
+          <t>1,324</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>2.034007352941177</v>
+        <v>1.605740181268882</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Phase II Garden B1</t>
+          <t>B2A</t>
         </is>
       </c>
       <c r="J19" t="b">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="O19" t="b">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Phase II Garden B1, $2,213 – $4,437, 2 beds, 2 baths, 1,088 – 1,143 sq ft, Tour This Floor Plan, View Phase II Garden B1, Floor Plan, View Phase II Garden B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Storage Units, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Crown Molding, Skylight, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 03610, price, $2,213, square feet, 1,143, availibility, Apr. 14, Unit 03610, Unit, 03502, price, $2,213, square feet, 1,143, availibility, May 19, Unit 03502, Unit, 03506, price, $2,213, square feet, 1,134, availibility, May 26, Unit 03506, </t>
+          <t xml:space="preserve">B2A, $2,126, 2 beds, 2 baths, 1,324 sq ft, Tour This Floor Plan, View B2A, Floor Plan, View B2A Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Views, Walk-In Closets, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 2109, price, $2,126, square feet, 1,324, availibility, Now, Unit 2109, </t>
         </is>
       </c>
     </row>
@@ -2094,40 +2094,40 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>St. Marin</t>
+          <t>Via Las Colinas</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/st-marin-coppell-tx/3mldpde/</t>
+          <t>https://www.apartments.com/via-las-colinas-irving-tx/m4vqwbj/</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1717 E Beltline Rd, Coppell, TX 75019</t>
+          <t>401 W Northwest Hwy, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Valley Ranch</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1,803</t>
+          <t>2,213</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1,263</t>
+          <t>1,088</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>1.427553444180523</v>
+        <v>2.034007352941177</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Bordeaux</t>
+          <t>Phase II Garden B1</t>
         </is>
       </c>
       <c r="J20" t="b">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="O20" t="b">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bordeaux, $1,803 – $4,373, 2 beds, 2 baths, 1,263 sq ft, Tour This Floor Plan, View Bordeaux, Floor Plan, View Bordeaux Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Fireplace, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Deck, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Recreation Room, Den, Built-In Bookshelves, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Window Coverings, 10 Available units, Unit, Price, Sq Ft, Availability, Unit, 02-0627, price, $1,803, square feet, 1,263, availibility, Now, Unit 02-0627, Unit, 01-0918, price, $1,878, square feet, 1,263, availibility, Now, Unit 01-0918, Unit, 02-0622, price, $1,893, square feet, 1,263, availibility, Now, Unit 02-0622, Show More Results (7), </t>
+          <t xml:space="preserve">Phase II Garden B1, $2,213 – $4,437, 2 beds, 2 baths, 1,088 – 1,143 sq ft, Tour This Floor Plan, View Phase II Garden B1, Floor Plan, View Phase II Garden B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Storage Units, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Crown Molding, Skylight, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 03610, price, $2,213, square feet, 1,143, availibility, Apr. 14, Unit 03610, Unit, 03502, price, $2,213, square feet, 1,143, availibility, May 19, Unit 03502, Unit, 03506, price, $2,213, square feet, 1,134, availibility, May 26, Unit 03506, </t>
         </is>
       </c>
     </row>
@@ -2180,47 +2180,47 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Las Colinas Heights Apartments</t>
+          <t>St. Marin</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/las-colinas-heights-apartments-irving-tx/p24w7jt/</t>
+          <t>https://www.apartments.com/st-marin-coppell-tx/3mldpde/</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3701 N Oconnor Rd, Irving, TX 75062</t>
+          <t>1717 E Beltline Rd, Coppell, TX 75019</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Valley Ranch</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>1,840</t>
+          <t>1,803</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1,335</t>
+          <t>1,263</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>1.378277153558052</v>
+        <v>1.427553444180523</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>B2 2x2</t>
+          <t>Bordeaux</t>
         </is>
       </c>
       <c r="J21" t="b">
         <v>1</v>
       </c>
       <c r="K21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" t="b">
         <v>1</v>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="O21" t="b">
@@ -2256,7 +2256,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2 2x2, $1,840 – $2,650, 2 beds, 2 baths, 1,335 sq ft, Available Now, Tour This Floor Plan, View B2 2x2, Floor Plan, View B2 2x2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Eat-in Kitchen, Kitchen, Microwave, Range, Refrigerator, Floor Plan Details, Balcony, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Walk-In Closets, Window Coverings, </t>
+          <t xml:space="preserve">Bordeaux, $1,803 – $4,373, 2 beds, 2 baths, 1,263 sq ft, Tour This Floor Plan, View Bordeaux, Floor Plan, View Bordeaux Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Fireplace, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Deck, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Recreation Room, Den, Built-In Bookshelves, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Window Coverings, 10 Available units, Unit, Price, Sq Ft, Availability, Unit, 02-0627, price, $1,803, square feet, 1,263, availibility, Now, Unit 02-0627, Unit, 01-0918, price, $1,878, square feet, 1,263, availibility, Now, Unit 01-0918, Unit, 02-0622, price, $1,893, square feet, 1,263, availibility, Now, Unit 02-0622, Show More Results (7), </t>
         </is>
       </c>
     </row>
@@ -2266,40 +2266,40 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Bridgeport</t>
+          <t>Las Colinas Heights Apartments</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/bridgeport-irving-tx/4eqtzyl/</t>
+          <t>https://www.apartments.com/las-colinas-heights-apartments-irving-tx/p24w7jt/</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4111 Polaris Dr, Irving, TX 75038</t>
+          <t>3701 N Oconnor Rd, Irving, TX 75062</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1,420</t>
+          <t>1,840</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>1,067</t>
+          <t>1,335</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>1.330834114339269</v>
+        <v>1.378277153558052</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B2 2x2</t>
         </is>
       </c>
       <c r="J22" t="b">
@@ -2338,11 +2338,11 @@
         <v>1</v>
       </c>
       <c r="U22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2, $1,420, 2 beds, 2 baths, 1,067 sq ft, $300 deposit, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Cable Ready, Storage Units, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Granite Countertops, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Recreation Room, Den, Sunroom, Walk-In Closets, Linen Closet, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 2-1108, price, $1,420, square feet, 1,067, availibility, Apr. 16, Unit 2-1108, </t>
+          <t xml:space="preserve">B2 2x2, $1,840 – $2,650, 2 beds, 2 baths, 1,335 sq ft, Available Now, Tour This Floor Plan, View B2 2x2, Floor Plan, View B2 2x2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Eat-in Kitchen, Kitchen, Microwave, Range, Refrigerator, Floor Plan Details, Balcony, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Walk-In Closets, Window Coverings, </t>
         </is>
       </c>
     </row>
@@ -2352,47 +2352,47 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Alesio Urban Center</t>
+          <t>Bridgeport</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/alesio-urban-center-irving-tx/ss6b8p7/</t>
+          <t>https://www.apartments.com/bridgeport-irving-tx/4eqtzyl/</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>385-385 E Las Colinas Blvd E, Irving, TX 75039</t>
+          <t>4111 Polaris Dr, Irving, TX 75038</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Urban Center Irving</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1,910</t>
+          <t>1,420</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>1,070</t>
+          <t>1,067</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>1.785046728971963</v>
+        <v>1.330834114339269</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Bella Villa X</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="J23" t="b">
         <v>1</v>
       </c>
       <c r="K23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" t="b">
         <v>1</v>
@@ -2402,7 +2402,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="O23" t="b">
@@ -2424,11 +2424,11 @@
         <v>1</v>
       </c>
       <c r="U23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bella Villa X, $1,910 – $2,655, 2 beds, 2 baths, 1,070 sq ft, 8 – 12 Month Lease, Tour This Floor Plan, View Bella Villa X, Floor Plan, View Bella Villa X Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Satellite TV, Security System, Storage Units, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Granite Countertops, Stainless Steel Appliances, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Built-In Bookshelves, Crown Molding, Vaulted Ceiling, Bay Window, Views, Walk-In Closets, Loft Layout, Window Coverings, Wet Bar, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 2629, price, $1,920, square feet, 1,070, availibility, Now, Unit 2629, Unit, 2315, price, $1,910, square feet, 1,070, availibility, Mar. 12, Unit 2315, </t>
+          <t xml:space="preserve">B2, $1,420, 2 beds, 2 baths, 1,067 sq ft, $300 deposit, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Cable Ready, Storage Units, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Granite Countertops, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Recreation Room, Den, Sunroom, Walk-In Closets, Linen Closet, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 2-1108, price, $1,420, square feet, 1,067, availibility, Apr. 16, Unit 2-1108, </t>
         </is>
       </c>
     </row>
@@ -2438,47 +2438,47 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Hyde Park at Valley Ranch</t>
+          <t>Alesio Urban Center</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/hyde-park-at-valley-ranch-irving-tx/mcvqd8l/</t>
+          <t>https://www.apartments.com/alesio-urban-center-irving-tx/ss6b8p7/</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>10201 N Macarthur Blvd, Irving, TX 75063</t>
+          <t>385-385 E Las Colinas Blvd E, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Valley Ranch</t>
+          <t>Urban Center Irving</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>1,705</t>
+          <t>1,910</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1,018</t>
+          <t>1,070</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>1.674852652259332</v>
+        <v>1.785046728971963</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2 Bd 2 Bth Renovated</t>
+          <t>Bella Villa X</t>
         </is>
       </c>
       <c r="J24" t="b">
         <v>1</v>
       </c>
       <c r="K24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" t="b">
         <v>1</v>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="O24" t="b">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 Bd 2 Bth Renovated, $1,705 – $2,030, 2 beds, 2 baths, 1,018 sq ft, $250 deposit, Tour This Floor Plan, View 2 Bd 2 Bth Renovated, Floor Plan, View 2 Bd 2 Bth Renovated Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Storage Units, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Porch, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Den, Built-In Bookshelves, Vaulted Ceiling, Walk-In Closets, Linen Closet, Window Coverings, Wet Bar, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 206-203, price, $1,705, square feet, 1,018, availibility, Apr. 16, Unit 206-203, Unit, 331-213, price, $1,705, square feet, 1,018, availibility, Apr. 16, Unit 331-213, Unit, 130-213, price, $1,715, square feet, 1,018, availibility, Apr. 16, Unit 130-213, </t>
+          <t xml:space="preserve">Bella Villa X, $1,910 – $2,655, 2 beds, 2 baths, 1,070 sq ft, 8 – 12 Month Lease, Tour This Floor Plan, View Bella Villa X, Floor Plan, View Bella Villa X Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Satellite TV, Security System, Storage Units, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Granite Countertops, Stainless Steel Appliances, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Built-In Bookshelves, Crown Molding, Vaulted Ceiling, Bay Window, Views, Walk-In Closets, Loft Layout, Window Coverings, Wet Bar, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 2629, price, $1,920, square feet, 1,070, availibility, Now, Unit 2629, Unit, 2315, price, $1,910, square feet, 1,070, availibility, Mar. 12, Unit 2315, </t>
         </is>
       </c>
     </row>
@@ -2524,47 +2524,47 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Apartments at the Sound</t>
+          <t>Hyde Park at Valley Ranch</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/apartments-at-the-sound-coppell-tx/4lwx78j/</t>
+          <t>https://www.apartments.com/hyde-park-at-valley-ranch-irving-tx/mcvqd8l/</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3203 Mulberry Hill Rd, Coppell, TX 75019</t>
+          <t>10201 N Macarthur Blvd, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Cypress Waters</t>
+          <t>Valley Ranch</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2,281</t>
+          <t>1,705</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1,188</t>
+          <t>1,018</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>1.92003367003367</v>
+        <v>1.674852652259332</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2 Bedroom, 2 Bath</t>
+          <t>2 Bd 2 Bth Renovated</t>
         </is>
       </c>
       <c r="J25" t="b">
         <v>1</v>
       </c>
       <c r="K25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" t="b">
         <v>1</v>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="O25" t="b">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 Bedroom, 2 Bath, $2,281 – $6,404, 2 beds, 2 baths, 1,188 sq ft, Available Now, Tour This Floor Plan, View 2 Bedroom, 2 Bath, Floor Plan, View 2 Bedroom, 2 Bath Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Intercom, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Porch, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Mud Room, Den, Built-In Bookshelves, Views, Walk-In Closets, Window Coverings, </t>
+          <t xml:space="preserve">2 Bd 2 Bth Renovated, $1,705 – $2,030, 2 beds, 2 baths, 1,018 sq ft, $250 deposit, Tour This Floor Plan, View 2 Bd 2 Bth Renovated, Floor Plan, View 2 Bd 2 Bth Renovated Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Storage Units, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Porch, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Den, Built-In Bookshelves, Vaulted Ceiling, Walk-In Closets, Linen Closet, Window Coverings, Wet Bar, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 206-203, price, $1,705, square feet, 1,018, availibility, Apr. 16, Unit 206-203, Unit, 331-213, price, $1,705, square feet, 1,018, availibility, Apr. 16, Unit 331-213, Unit, 130-213, price, $1,715, square feet, 1,018, availibility, Apr. 16, Unit 130-213, </t>
         </is>
       </c>
     </row>
@@ -2610,47 +2610,47 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Riverside Park</t>
+          <t>Apartments at the Sound</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/riverside-park-farmers-branch-tx/5qkvldp/</t>
+          <t>https://www.apartments.com/apartments-at-the-sound-coppell-tx/4lwx78j/</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1521 E Royal Ln, Farmers Branch, TX 75234</t>
+          <t>3203 Mulberry Hill Rd, Coppell, TX 75019</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Farmers Branch</t>
+          <t>Cypress Waters</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2,350</t>
+          <t>2,281</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1,117</t>
+          <t>1,188</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>2.103849597135183</v>
+        <v>1.92003367003367</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>B5</t>
+          <t>2 Bedroom, 2 Bath</t>
         </is>
       </c>
       <c r="J26" t="b">
         <v>1</v>
       </c>
       <c r="K26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" t="b">
         <v>1</v>
@@ -2660,7 +2660,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="O26" t="b">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t xml:space="preserve">B5, $2,350 – $3,317, 2 beds, 2 baths, Tour This Floor Plan, View B5, Floor Plan, View B5 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Security System, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Dining Room, Office, Den, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1212, price, $2,350, square feet, 1,117, availibility, Now, Unit 1212, </t>
+          <t xml:space="preserve">2 Bedroom, 2 Bath, $2,281 – $6,404, 2 beds, 2 baths, 1,188 sq ft, Available Now, Tour This Floor Plan, View 2 Bedroom, 2 Bath, Floor Plan, View 2 Bedroom, 2 Bath Floor Plan Details, Show Floor Plan Details, </t>
         </is>
       </c>
     </row>
@@ -2696,47 +2696,47 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>The Stations at MacArthur</t>
+          <t>Riverside Park</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/the-stations-at-macarthur-irving-tx/p95s9nv/</t>
+          <t>https://www.apartments.com/riverside-park-farmers-branch-tx/5qkvldp/</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1100 Hidden Ridge Dr, Irving, TX 75038</t>
+          <t>1521 E Royal Ln, Farmers Branch, TX 75234</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Farmers Branch</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2,083</t>
+          <t>2,350</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1,256</t>
+          <t>1,117</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>1.65843949044586</v>
+        <v>2.103849597135183</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B5</t>
         </is>
       </c>
       <c r="J27" t="b">
         <v>1</v>
       </c>
       <c r="K27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" t="b">
         <v>1</v>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="O27" t="b">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t xml:space="preserve">B3, $2,083 – $2,338, 2 beds, 2 baths, 1,256 sq ft, $250 deposit, Tour This Floor Plan, View B3, Floor Plan, View B3 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Ceiling Fans, Smoke Free, Cable Ready, Security System, Fireplace, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Kitchen, Microwave, Oven, Refrigerator, Freezer, Floor Plan Details, Balcony, Yard, Hardwood Floors, Carpet, Crown Molding, Views, Skylight, Walk-In Closets, Window Coverings, Large Bedrooms, 7 Available units, Unit, Price, Sq Ft, Availability, Unit, 2391, price, $2,288, square feet, 1,256, availibility, Now, Unit 2391, Unit, 2333, price, $2,233, square feet, 1,256, availibility, Mar. 18, Unit 2333, Unit, 2249, price, $2,263, square feet, 1,256, availibility, Mar. 23, Unit 2249, Show More Results (4), </t>
+          <t xml:space="preserve">B5, $2,350 – $3,317, 2 beds, 2 baths, Tour This Floor Plan, View B5, Floor Plan, View B5 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Security System, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Dining Room, Office, Den, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1212, price, $2,350, square feet, 1,117, availibility, Now, Unit 1212, </t>
         </is>
       </c>
     </row>
@@ -2782,40 +2782,40 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Lux on Main</t>
+          <t>The Stations at MacArthur</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/lux-on-main-carrollton-tx/ze5j4dy/</t>
+          <t>https://www.apartments.com/the-stations-at-macarthur-irving-tx/p95s9nv/</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1011 S Main St, Carrollton, TX 75006</t>
+          <t>1100 Hidden Ridge Dr, Irving, TX 75038</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Carrollton</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2,350</t>
+          <t>2,083</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>1,070</t>
+          <t>1,256</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>2.196261682242991</v>
+        <v>1.65843949044586</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="J28" t="b">
@@ -2832,7 +2832,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="O28" t="b">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $2,350, 2 beds, 2 baths, 1,070 sq ft, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Satellite TV, Trash Compactor, Storage Units, Tub/Shower, Handrails, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Instant Hot Water, Floor Plan Details, Balcony, Patio, Carpet, Tile Floors, Vinyl Flooring, Office, Den, Walk-In Closets, Linen Closet, Double Pane Windows, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 4520, price, $2,350, square feet, 1,070, availibility, Now, Unit 4520, </t>
+          <t xml:space="preserve">B3, $2,083 – $2,338, 2 beds, 2 baths, 1,256 sq ft, $250 deposit, Tour This Floor Plan, View B3, Floor Plan, View B3 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Ceiling Fans, Smoke Free, Cable Ready, Security System, Fireplace, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Kitchen, Microwave, Oven, Refrigerator, Freezer, Floor Plan Details, Balcony, Yard, Hardwood Floors, Carpet, Crown Molding, Views, Skylight, Walk-In Closets, Window Coverings, Large Bedrooms, 7 Available units, Unit, Price, Sq Ft, Availability, Unit, 2391, price, $2,288, square feet, 1,256, availibility, Now, Unit 2391, Unit, 2333, price, $2,233, square feet, 1,256, availibility, Mar. 18, Unit 2333, Unit, 2249, price, $2,263, square feet, 1,256, availibility, Mar. 23, Unit 2249, Show More Results (4), </t>
         </is>
       </c>
     </row>
@@ -2868,40 +2868,40 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Eastshore on Lake Carolyn</t>
+          <t>Lux on Main</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/eastshore-on-lake-carolyn-irving-tx/0sb0q61/</t>
+          <t>https://www.apartments.com/lux-on-main-carrollton-tx/ze5j4dy/</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1100 Lake Carolyn Pky, Irving, TX 75039</t>
+          <t>1011 S Main St, Carrollton, TX 75006</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Urban Center Irving</t>
+          <t>Carrollton</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2,200</t>
+          <t>2,350</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>1,171</t>
+          <t>1,070</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>1.878736122971819</v>
+        <v>2.196261682242991</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>B2E</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J29" t="b">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="O29" t="b">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2E, $2,200 – $3,834, 2 beds, 2 baths, 1,171 sq ft, Available Now, Tour This Floor Plan, View B2E, Floor Plan, View B2E Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Double Vanities, Tub/Shower, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Mud Room, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, </t>
+          <t xml:space="preserve">B1, $2,350, 2 beds, 2 baths, 1,070 sq ft, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Satellite TV, Trash Compactor, Storage Units, Tub/Shower, Handrails, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Instant Hot Water, Floor Plan Details, Balcony, Patio, Carpet, Tile Floors, Vinyl Flooring, Office, Den, Walk-In Closets, Linen Closet, Double Pane Windows, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 4520, price, $2,350, square feet, 1,070, availibility, Now, Unit 4520, </t>
         </is>
       </c>
     </row>
@@ -2954,17 +2954,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Promenade at Las Colinas</t>
+          <t>Eastshore on Lake Carolyn</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/promenade-at-las-colinas-irving-tx/xjx6z4p/</t>
+          <t>https://www.apartments.com/eastshore-on-lake-carolyn-irving-tx/0sb0q61/</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>555 Promenade Pky, Irving, TX 75039</t>
+          <t>1100 Lake Carolyn Pky, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2974,20 +2974,20 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2,245</t>
+          <t>2,200</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>1,161</t>
+          <t>1,171</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>1.933677863910422</v>
+        <v>1.878736122971819</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>B2C</t>
+          <t>B2E</t>
         </is>
       </c>
       <c r="J30" t="b">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="O30" t="b">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2C, $2,245 – $3,774, 2 beds, 2 baths, 1,161 sq ft, Tour This Floor Plan, View B2C, Floor Plan, View B2C, Virtual Tours, View B2C Floor Plan Details, Hide Floor Plan Details, Highlights, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Yard, Garden, Hardwood Floors, Carpet, Vinyl Flooring, Office, Den, Built-In Bookshelves, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Loft Layout, Double Pane Windows, Window Coverings, Large Bedrooms, 4 Available units, Unit, Price, Sq Ft, Availability, Unit, 175, price, $2,375, square feet, 1,161, availibility, Now, Unit 175, Unit, 404, price, $2,265, square feet, 1,161, availibility, Mar. 11, Unit 404, Unit, 475, price, $2,245, square feet, 1,161, availibility, Apr. 9, Unit 475, Show More Results (1), </t>
+          <t xml:space="preserve">B2E, $2,200 – $3,834, 2 beds, 2 baths, 1,171 sq ft, Available Now, Tour This Floor Plan, View B2E, Floor Plan, View B2E Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Double Vanities, Tub/Shower, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Mud Room, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, </t>
         </is>
       </c>
     </row>
@@ -3040,17 +3040,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Gables Water Street</t>
+          <t>Promenade at Las Colinas</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/gables-water-street-irving-tx/8v0t9l1/</t>
+          <t>https://www.apartments.com/promenade-at-las-colinas-irving-tx/xjx6z4p/</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>5270 N O'Connor Blvd, Irving, TX 75039</t>
+          <t>555 Promenade Pky, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -3060,20 +3060,20 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2,805</t>
+          <t>2,245</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>1,164</t>
+          <t>1,161</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>2.40979381443299</v>
+        <v>1.933677863910422</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>B2-B</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="J31" t="b">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="O31" t="b">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2-B, $2,805 – $4,831, 2 beds, 2 baths, 1,164 sq ft, Tour This Floor Plan, View B2-B, Floor Plan, View B2-B Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Vinyl Flooring, Built-In Bookshelves, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1524, price, $2,805, square feet, 1,164, availibility, Now, Unit 1524, </t>
+          <t xml:space="preserve">B2C, $2,245 – $3,774, 2 beds, 2 baths, 1,161 sq ft, Tour This Floor Plan, View B2C, Floor Plan, View B2C, Virtual Tours, View B2C Floor Plan Details, Hide Floor Plan Details, Highlights, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Yard, Garden, Hardwood Floors, Carpet, Vinyl Flooring, Office, Den, Built-In Bookshelves, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Loft Layout, Double Pane Windows, Window Coverings, Large Bedrooms, 4 Available units, Unit, Price, Sq Ft, Availability, Unit, 175, price, $2,375, square feet, 1,161, availibility, Now, Unit 175, Unit, 404, price, $2,265, square feet, 1,161, availibility, Mar. 11, Unit 404, Unit, 475, price, $2,245, square feet, 1,161, availibility, Apr. 9, Unit 475, Show More Results (1), </t>
         </is>
       </c>
     </row>
@@ -3126,17 +3126,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>AMLI Campion Trail</t>
+          <t>Gables Water Street</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/amli-campion-trail-irving-tx/9pfk0z7/</t>
+          <t>https://www.apartments.com/gables-water-street-irving-tx/8v0t9l1/</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>777 Lake Carolyn Pky, Irving, TX 75039</t>
+          <t>5270 N O'Connor Blvd, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -3146,20 +3146,20 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2,138</t>
+          <t>2,805</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>1,211</t>
+          <t>1,164</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>1.765483071841453</v>
+        <v>2.40979381443299</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>C6</t>
+          <t>B2-B</t>
         </is>
       </c>
       <c r="J32" t="b">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="O32" t="b">
@@ -3202,7 +3202,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t xml:space="preserve">C6, $2,138 – $2,884, 2 beds, 2 baths, 1,211 sq ft, $500 deposit, Available Now, Tour This Floor Plan, View C6, Floor Plan, View C6 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Den, Built-In Bookshelves, Crown Molding, Views, Walk-In Closets, Linen Closet, Furnished, Window Coverings, Large Bedrooms, </t>
+          <t xml:space="preserve">B2-B, $2,805 – $4,831, 2 beds, 2 baths, 1,164 sq ft, Tour This Floor Plan, View B2-B, Floor Plan, View B2-B Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Vinyl Flooring, Built-In Bookshelves, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1524, price, $2,805, square feet, 1,164, availibility, Now, Unit 1524, </t>
         </is>
       </c>
     </row>
@@ -3212,40 +3212,40 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Rancho Mirage</t>
+          <t>AMLI Campion Trail</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/rancho-mirage-irving-tx/r1jp4s2/</t>
+          <t>https://www.apartments.com/amli-campion-trail-irving-tx/9pfk0z7/</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1200 Hidden Rdg, Irving, TX 75038</t>
+          <t>777 Lake Carolyn Pky, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Urban Center Irving</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>1,972</t>
+          <t>2,138</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>1,243</t>
+          <t>1,211</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>1.586484312148029</v>
+        <v>1.765483071841453</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2 Bedroom 2 Bath B</t>
+          <t>C6</t>
         </is>
       </c>
       <c r="J33" t="b">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 Bedroom 2 Bath B, $1,972 – $2,371, 2 beds, 2 baths, 1,243 sq ft, $200 deposit, Tour This Floor Plan, View 2 Bedroom 2 Bath B, Floor Plan, View 2 Bedroom 2 Bath B Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Security System, Trash Compactor, Storage Units, Tub/Shower, Fireplace, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Deck, Carpet, Vinyl Flooring, Dining Room, Den, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 2085, price, $1,972, square feet, 1,243, availibility, Mar. 17, Unit 2085, </t>
+          <t xml:space="preserve">C6, $2,138 – $2,884, 2 beds, 2 baths, 1,211 sq ft, $500 deposit, Available Now, Tour This Floor Plan, View C6, Floor Plan, View C6 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Den, Built-In Bookshelves, Crown Molding, Views, Walk-In Closets, Linen Closet, Furnished, Window Coverings, Large Bedrooms, </t>
         </is>
       </c>
     </row>
@@ -3298,40 +3298,40 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Switchyard</t>
+          <t>Rancho Mirage</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/switchyard-carrollton-tx/nfecnln/</t>
+          <t>https://www.apartments.com/rancho-mirage-irving-tx/r1jp4s2/</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1199 N Broadway St, Carrollton, TX 75006</t>
+          <t>1200 Hidden Rdg, Irving, TX 75038</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Downtown Carrollton</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2,070</t>
+          <t>1,972</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>953</t>
+          <t>1,243</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>2.17208814270724</v>
+        <v>1.586484312148029</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>2 Bedroom 2 Bath B</t>
         </is>
       </c>
       <c r="J34" t="b">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="O34" t="b">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $2,070 – $2,145, 2 beds, 2 baths, 953 sq ft, Available Now, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Deck, Carpet, Vinyl Flooring, Family Room, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, </t>
+          <t xml:space="preserve">2 Bedroom 2 Bath B, $1,972 – $2,371, 2 beds, 2 baths, 1,243 sq ft, $200 deposit, Tour This Floor Plan, View 2 Bedroom 2 Bath B, Floor Plan, View 2 Bedroom 2 Bath B Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Security System, Trash Compactor, Storage Units, Tub/Shower, Fireplace, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Deck, Carpet, Vinyl Flooring, Dining Room, Den, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 2085, price, $1,972, square feet, 1,243, availibility, Mar. 17, Unit 2085, </t>
         </is>
       </c>
     </row>
@@ -3384,36 +3384,36 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Cayman Las Colinas</t>
+          <t>Switchyard</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/cayman-las-colinas-irving-tx/ljhtdrg/</t>
+          <t>https://www.apartments.com/switchyard-carrollton-tx/nfecnln/</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1071 Lake Carolyn Pky, Irving, TX 75039</t>
+          <t>1199 N Broadway St, Carrollton, TX 75006</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Downtown Carrollton</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>1,999</t>
+          <t>2,070</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>973</t>
+          <t>953</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>2.054470709146968</v>
+        <v>2.17208814270724</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="O35" t="b">
@@ -3460,7 +3460,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $1,999, 2 beds, 2 baths, 973 sq ft, 3 – 15 Month Lease,$250 deposit, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Satellite TV, Security System, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Fireplace, Handrails, Surround Sound, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Warming Drawer, Instant Hot Water, Floor Plan Details, Balcony, Patio, Porch, Deck, Yard, Lawn, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Family Room, Mud Room, Office, Recreation Room, Sunroom, Built-In Bookshelves, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Loft Layout, Double Pane Windows, Window Coverings, Wet Bar, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1063, price, $1,999, square feet, 973, availibility, Apr. 26, Unit 1063, </t>
+          <t xml:space="preserve">B1, $2,070 – $2,145, 2 beds, 2 baths, 953 sq ft, Available Now, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Tub/Shower, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Deck, Carpet, Vinyl Flooring, Family Room, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, </t>
         </is>
       </c>
     </row>
@@ -3470,47 +3470,47 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>The Trails of Valley Ranch</t>
+          <t>Cayman Las Colinas</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/the-trails-of-valley-ranch-irving-tx/1w11g96/</t>
+          <t>https://www.apartments.com/cayman-las-colinas-irving-tx/ljhtdrg/</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>9478 E Valley Ranch Pky E, Irving, TX 75063</t>
+          <t>1071 Lake Carolyn Pky, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Valley Ranch</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>1,659</t>
+          <t>1,999</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>936</t>
+          <t>973</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>1.772435897435897</v>
+        <v>2.054470709146968</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J36" t="b">
         <v>1</v>
       </c>
       <c r="K36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" t="b">
         <v>1</v>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="O36" t="b">
@@ -3546,7 +3546,7 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2, $1,659 – $1,879, 2 beds, 2 baths, 936 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Storage Units, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Walk-In Closets, Window Coverings, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 1012, price, $1,659, square feet, 936, availibility, May 7, Unit 1012, Unit, 1044, price, $1,659, square feet, 936, availibility, May 20, Unit 1044, </t>
+          <t xml:space="preserve">B1, $1,999, 2 beds, 2 baths, 973 sq ft, 3 – 15 Month Lease,$250 deposit, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Satellite TV, Security System, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Fireplace, Handrails, Surround Sound, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Warming Drawer, Instant Hot Water, Floor Plan Details, Balcony, Patio, Porch, Deck, Yard, Lawn, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Family Room, Mud Room, Office, Recreation Room, Sunroom, Built-In Bookshelves, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Loft Layout, Double Pane Windows, Window Coverings, Wet Bar, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1063, price, $1,999, square feet, 973, availibility, Apr. 26, Unit 1063, </t>
         </is>
       </c>
     </row>
@@ -3556,47 +3556,47 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Lakeside Lofts</t>
+          <t>The Trails of Valley Ranch</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/lakeside-lofts-farmers-branch-tx/ndph2tp/</t>
+          <t>https://www.apartments.com/the-trails-of-valley-ranch-irving-tx/1w11g96/</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>11500 Lago Vista E, Farmers Branch, TX 75234</t>
+          <t>9478 E Valley Ranch Pky E, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Koreatown/Gribble</t>
+          <t>Valley Ranch</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>1,904</t>
+          <t>1,659</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>1,106</t>
+          <t>936</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>1.721518987341772</v>
+        <v>1.772435897435897</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="J37" t="b">
         <v>1</v>
       </c>
       <c r="K37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37" t="b">
         <v>1</v>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="O37" t="b">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $1,904 – $2,074, 2 beds, 2 baths, 1,106 sq ft, Tour This Floor Plan, View B1, Floor Plan, View B1, Virtual Tours, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Double Vanities, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Porch, Yard, Lawn, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Recreation Room, Den, Crown Molding, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 16 Available units, Unit, Price, Sq Ft, Availability, Unit, 1238, price, $2,009, square feet, 1,106, availibility, Now, Unit 1238, Unit, 2351, price, $2,049, square feet, 1,106, availibility, Mar. 31, Unit 2351, Unit, 1234, price, $2,009, square feet, 1,106, availibility, Apr. 7, Unit 1234, Show More Results (13), </t>
+          <t xml:space="preserve">B2, $1,659 – $1,879, 2 beds, 2 baths, 936 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Storage Units, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Walk-In Closets, Window Coverings, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 1012, price, $1,659, square feet, 936, availibility, May 7, Unit 1012, Unit, 1044, price, $1,659, square feet, 936, availibility, May 20, Unit 1044, </t>
         </is>
       </c>
     </row>
@@ -3642,47 +3642,47 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MacArthur Ridge Apartments</t>
+          <t>Lakeside Lofts</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/macarthur-ridge-apartments-irving-tx/4g9dz7h/</t>
+          <t>https://www.apartments.com/lakeside-lofts-farmers-branch-tx/ndph2tp/</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>10701 N MacArthur Blvd, Irving, TX 75063</t>
+          <t>11500 Lago Vista E, Farmers Branch, TX 75234</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Valley Ranch</t>
+          <t>Koreatown/Gribble</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>1,668</t>
+          <t>1,904</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>984</t>
+          <t>1,106</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>1.695121951219512</v>
+        <v>1.721518987341772</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Elm</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J38" t="b">
         <v>1</v>
       </c>
       <c r="K38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" t="b">
         <v>1</v>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>NONE</t>
         </is>
       </c>
       <c r="O38" t="b">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Elm, $1,668 – $3,216, 2 beds, 2 baths, 984 sq ft, Mar. 11, Tour This Floor Plan, View Elm, Floor Plan, View Elm Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Walk-In Closets, Window Coverings, </t>
+          <t xml:space="preserve">B1, $1,904 – $2,074, 2 beds, 2 baths, 1,106 sq ft, Tour This Floor Plan, View B1, Floor Plan, View B1, Virtual Tours, View B1 Floor Plan Details, Show Floor Plan Details, 16 Available units, Unit, Price, Sq Ft, Availability, Unit, 1238, price, $2,009, square feet, 1,106, availibility, Now, Unit 1238, Unit, 2351, price, $2,049, square feet, 1,106, availibility, Mar. 31, Unit 2351, Unit, 1234, price, $2,009, square feet, 1,106, availibility, Apr. 7, Unit 1234, Show More Results (13), </t>
         </is>
       </c>
     </row>
@@ -3728,47 +3728,47 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Calloway at Las Colinas</t>
+          <t>MacArthur Ridge Apartments</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/calloway-at-las-colinas-irving-tx/rsrsxc1/</t>
+          <t>https://www.apartments.com/macarthur-ridge-apartments-irving-tx/4g9dz7h/</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7300 Parkridge Blvd, Irving, TX 75063</t>
+          <t>10701 N MacArthur Blvd, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Valley Ranch</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>1,810</t>
+          <t>1,668</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>1,100</t>
+          <t>984</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>1.645454545454546</v>
+        <v>1.695121951219512</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Gardenia 2x2</t>
+          <t>Elm</t>
         </is>
       </c>
       <c r="J39" t="b">
         <v>1</v>
       </c>
       <c r="K39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39" t="b">
         <v>1</v>
@@ -3804,7 +3804,7 @@
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gardenia 2x2, $1,810 – $3,066, 2 beds, 2 baths, 1,100 sq ft, Apr. 1, Tour This Floor Plan, View Gardenia 2x2, Floor Plan, View Gardenia 2x2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Family Room, Recreation Room, Walk-In Closets, Window Coverings, Large Bedrooms, </t>
+          <t xml:space="preserve">Elm, $1,668 – $3,216, 2 beds, 2 baths, 984 sq ft, Mar. 11, Tour This Floor Plan, View Elm, Floor Plan, View Elm Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Walk-In Closets, Window Coverings, </t>
         </is>
       </c>
     </row>
@@ -3814,17 +3814,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>MacArthur Park</t>
+          <t>Calloway at Las Colinas</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/macarthur-park-irving-tx/gn0wrmy/</t>
+          <t>https://www.apartments.com/calloway-at-las-colinas-irving-tx/rsrsxc1/</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>812 Kinwest, Irving, TX 75063</t>
+          <t>7300 Parkridge Blvd, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -3834,7 +3834,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>1,675</t>
+          <t>1,810</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -3843,11 +3843,11 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>1.522727272727273</v>
+        <v>1.645454545454546</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Two Bed / Two Bath</t>
+          <t>Gardenia 2x2</t>
         </is>
       </c>
       <c r="J40" t="b">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="O40" t="b">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Two Bed / Two Bath, $1,675 – $1,685, 2 beds, 2 baths, 1,100 sq ft, $250 deposit, Tour This Floor Plan, View Two Bed / Two Bath, Floor Plan, View Two Bed / Two Bath, Virtual Tours, View Two Bed / Two Bath Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Trash Compactor, Storage Units, Tub/Shower, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Kitchen, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Vaulted Ceiling, Views, Walk-In Closets, Window Coverings, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 124, price, $1,685, square feet, 1,100, availibility, Apr. 16, Unit 124, Unit, 104, price, $1,675, square feet, 1,100, availibility, Apr. 30, Unit 104, Unit, 107, price, $1,685, square feet, 1,100, availibility, May 21, Unit 107, </t>
+          <t xml:space="preserve">Gardenia 2x2, $1,810 – $3,066, 2 beds, 2 baths, 1,100 sq ft, Apr. 1, Tour This Floor Plan, View Gardenia 2x2, Floor Plan, View Gardenia 2x2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Family Room, Recreation Room, Walk-In Closets, Window Coverings, Large Bedrooms, </t>
         </is>
       </c>
     </row>
@@ -3900,47 +3900,47 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Avalon 8801</t>
+          <t>MacArthur Park</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/avalon-8801-irving-tx/frgsjkr/</t>
+          <t>https://www.apartments.com/macarthur-park-irving-tx/gn0wrmy/</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>8801 Rodeo Dr, Irving, TX 75063</t>
+          <t>812 Kinwest, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Valley Ranch</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>1,783</t>
+          <t>1,675</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>959</t>
+          <t>1,100</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>1.859228362877998</v>
+        <v>1.522727272727273</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>The Rio Grande</t>
+          <t>Two Bed / Two Bath</t>
         </is>
       </c>
       <c r="J41" t="b">
         <v>1</v>
       </c>
       <c r="K41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" t="b">
         <v>1</v>
@@ -3950,7 +3950,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="O41" t="b">
@@ -3972,11 +3972,11 @@
         <v>1</v>
       </c>
       <c r="U41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Rio Grande, $1,783, 2 beds, 2 baths, 959 sq ft, Available Now, Tour This Floor Plan, View The Rio Grande, Floor Plan, View The Rio Grande Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Storage Units, Tub/Shower, Fireplace, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Breakfast Nook, Instant Hot Water, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Den, Built-In Bookshelves, Crown Molding, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Window Coverings, </t>
+          <t xml:space="preserve">Two Bed / Two Bath, $1,675 – $1,685, 2 beds, 2 baths, 1,100 sq ft, $250 deposit, Tour This Floor Plan, View Two Bed / Two Bath, Floor Plan, View Two Bed / Two Bath, Virtual Tours, View Two Bed / Two Bath Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Trash Compactor, Storage Units, Tub/Shower, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Kitchen, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Vaulted Ceiling, Views, Walk-In Closets, Window Coverings, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 124, price, $1,685, square feet, 1,100, availibility, Apr. 16, Unit 124, Unit, 104, price, $1,675, square feet, 1,100, availibility, Apr. 30, Unit 104, Unit, 107, price, $1,685, square feet, 1,100, availibility, May 21, Unit 107, </t>
         </is>
       </c>
     </row>
@@ -3986,47 +3986,47 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Boardwalk at Mercer Crossing</t>
+          <t>Avalon 8801</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/boardwalk-at-mercer-crossing-farmers-branch-tx/nbhsd6q/</t>
+          <t>https://www.apartments.com/avalon-8801-irving-tx/frgsjkr/</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1901 Knightsbridge Rd, Farmers Branch, TX 75234</t>
+          <t>8801 Rodeo Dr, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Koreatown/Gribble</t>
+          <t>Valley Ranch</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>1,981</t>
+          <t>1,783</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>1,150</t>
+          <t>959</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>1.722608695652174</v>
+        <v>1.859228362877998</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>B2B</t>
+          <t>The Rio Grande</t>
         </is>
       </c>
       <c r="J42" t="b">
         <v>1</v>
       </c>
       <c r="K42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" t="b">
         <v>1</v>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="O42" t="b">
@@ -4058,11 +4058,11 @@
         <v>1</v>
       </c>
       <c r="U42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2B, $1,981 – $2,862, 2 beds, 2 baths, 1,150 sq ft, Tour This Floor Plan, View B2B, Floor Plan, View B2B Floor Plan Details, Hide Floor Plan Details, Highlights, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Double Vanities, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Office, Den, Views, Walk-In Closets, Linen Closet, Loft Layout, Double Pane Windows, Window Coverings, Large Bedrooms, 4 Available units, Unit, Price, Sq Ft, Availability, Unit, 10310, price, $1,981, square feet, 1,150, availibility, Now, Unit 10310, Unit, 06305, price, $1,981, square feet, 1,150, availibility, Now, Unit 06305, Unit, 02208, price, $2,071, square feet, 1,150, availibility, Now, Unit 02208, Show More Results (1), </t>
+          <t xml:space="preserve">The Rio Grande, $1,783, 2 beds, 2 baths, 959 sq ft, Available Now, Tour This Floor Plan, View The Rio Grande, Floor Plan, View The Rio Grande Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Storage Units, Tub/Shower, Fireplace, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Breakfast Nook, Instant Hot Water, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Den, Built-In Bookshelves, Crown Molding, Vaulted Ceiling, Views, Walk-In Closets, Linen Closet, Window Coverings, </t>
         </is>
       </c>
     </row>
@@ -4072,40 +4072,40 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Monterra Las Colinas Apartments</t>
+          <t>Boardwalk at Mercer Crossing</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/monterra-las-colinas-apartments-irving-tx/2ww05yc/</t>
+          <t>https://www.apartments.com/boardwalk-at-mercer-crossing-farmers-branch-tx/nbhsd6q/</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>301 W Las Colinas Blvd W, Irving, TX 75039</t>
+          <t>1901 Knightsbridge Rd, Farmers Branch, TX 75234</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Urban Center Irving</t>
+          <t>Koreatown/Gribble</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1,700</t>
+          <t>1,981</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>1,025</t>
+          <t>1,150</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>1.658536585365854</v>
+        <v>1.722608695652174</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="J43" t="b">
@@ -4122,7 +4122,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="O43" t="b">
@@ -4148,7 +4148,7 @@
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $1,700 – $1,800, 2 beds, 2 baths, 1,025 sq ft, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Office, Den, Built-In Bookshelves, Vaulted Ceiling, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, C-324, price, $1,800, square feet, 1,025, availibility, Now, Unit C-324, Unit, E-152, price, $1,700, square feet, 1,025, availibility, May 7, Unit E-152, </t>
+          <t xml:space="preserve">B2B, $1,981 – $2,862, 2 beds, 2 baths, 1,150 sq ft, Tour This Floor Plan, View B2B, Floor Plan, View B2B Floor Plan Details, Hide Floor Plan Details, Highlights, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Double Vanities, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Vinyl Flooring, Office, Den, Views, Walk-In Closets, Linen Closet, Loft Layout, Double Pane Windows, Window Coverings, Large Bedrooms, 4 Available units, Unit, Price, Sq Ft, Availability, Unit, 10310, price, $1,981, square feet, 1,150, availibility, Now, Unit 10310, Unit, 06305, price, $1,981, square feet, 1,150, availibility, Now, Unit 06305, Unit, 02208, price, $2,071, square feet, 1,150, availibility, Now, Unit 02208, Show More Results (1), </t>
         </is>
       </c>
     </row>
@@ -4158,40 +4158,40 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Tides on Ranchview</t>
+          <t>Monterra Las Colinas Apartments</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/tides-on-ranchview-irving-tx/f1s6ggv/</t>
+          <t>https://www.apartments.com/monterra-las-colinas-apartments-irving-tx/2ww05yc/</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>8203 Ranchview Dr, Irving, TX 75063</t>
+          <t>301 W Las Colinas Blvd W, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Urban Center Irving</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>1,895</t>
+          <t>1,700</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>1,140</t>
+          <t>1,025</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>1.662280701754386</v>
+        <v>1.658536585365854</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>8217 Ranchview Dr #2002</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J44" t="b">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="O44" t="b">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t xml:space="preserve">8217 Ranchview Dr #2002, $1,895, 2 beds, 2 baths, 1,140 sq ft, Mar. 15, Tour This Floor Plan, View 8217 Ranchview Dr #2002 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Fireplace, Handrails, Sprinkler System, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Recreation Room, Den, Crown Molding, Walk-In Closets, Window Coverings, </t>
+          <t xml:space="preserve">B1, $1,700 – $1,800, 2 beds, 2 baths, 1,025 sq ft, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Tub/Shower, Fireplace, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Office, Den, Built-In Bookshelves, Vaulted Ceiling, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, C-324, price, $1,800, square feet, 1,025, availibility, Now, Unit C-324, Unit, E-152, price, $1,700, square feet, 1,025, availibility, May 7, Unit E-152, </t>
         </is>
       </c>
     </row>
@@ -4244,40 +4244,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Avalon Villas</t>
+          <t>Tides on Ranchview</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/avalon-villas-irving-tx/2mt2n5b/</t>
+          <t>https://www.apartments.com/tides-on-ranchview-irving-tx/f1s6ggv/</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>4447 Rainier St, Irving, TX 75062</t>
+          <t>8203 Ranchview Dr, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>1,619</t>
+          <t>1,895</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>1,150</t>
+          <t>1,140</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>1.407826086956522</v>
+        <v>1.662280701754386</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>8217 Ranchview Dr #2002</t>
         </is>
       </c>
       <c r="J45" t="b">
@@ -4294,14 +4294,14 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="O45" t="b">
         <v>1</v>
       </c>
       <c r="P45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q45" t="b">
         <v>1</v>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t xml:space="preserve">B3, $1,619 – $1,699, 2 beds, 2 baths, 1,150 sq ft, Tour This Floor Plan, View B3, Floor Plan, View B3 Floor Plan Details, Hide Floor Plan Details, Features, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Smoke Free, Fireplace, Dishwasher, Balcony, Patio, Carpet, Sunroom, Walk-In Closets, 8 Available units, Unit, Price, Sq Ft, Availability, Unit, 194, price, $1,619, square feet, 1,150, availibility, Now, Unit 194, Unit, 105, price, $1,619, square feet, 1,150, availibility, Now, Unit 105, Unit, 245, price, $1,699, square feet, 1,150, availibility, Mar. 16, Unit 245, Show More Results (5), </t>
+          <t xml:space="preserve">8217 Ranchview Dr #2002, $1,895, 2 beds, 2 baths, 1,140 sq ft, Mar. 15, Tour This Floor Plan, View 8217 Ranchview Dr #2002 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Fireplace, Handrails, Sprinkler System, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Recreation Room, Den, Crown Molding, Walk-In Closets, Window Coverings, </t>
         </is>
       </c>
     </row>
@@ -4330,36 +4330,36 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Dominion at Mercer Crossing</t>
+          <t>Avalon Villas</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/dominion-at-mercer-crossing-farmers-branch-tx/6rgqd5v/</t>
+          <t>https://www.apartments.com/avalon-villas-irving-tx/2mt2n5b/</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>11771 Mira Lago Blvd, Farmers Branch, TX 75234</t>
+          <t>4447 Rainier St, Irving, TX 75062</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Northwest Dallas</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2,019</t>
+          <t>1,619</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>1,295</t>
+          <t>1,150</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>1.559073359073359</v>
+        <v>1.407826086956522</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -4380,14 +4380,14 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="O46" t="b">
         <v>1</v>
       </c>
       <c r="P46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q46" t="b">
         <v>1</v>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t xml:space="preserve">B3, $2,019 – $2,049, 2 beds, 2 baths, 1,295 sq ft, Tour This Floor Plan, View B3, Floor Plan, View B3 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Satellite TV, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Porch, Deck, Yard, Hardwood Floors, Carpet, Dining Room, Walk-In Closets, Double Pane Windows, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 1243, price, $2,019, square feet, 1,295, availibility, Now, Unit 1243, Unit, 1204, price, $2,049, square feet, 1,295, availibility, Apr. 8, Unit 1204, </t>
+          <t xml:space="preserve">B3, $1,619 – $1,699, 2 beds, 2 baths, 1,150 sq ft, Tour This Floor Plan, View B3, Floor Plan, View B3 Floor Plan Details, Hide Floor Plan Details, Features, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Smoke Free, Fireplace, Dishwasher, Balcony, Patio, Carpet, Sunroom, Walk-In Closets, 8 Available units, Unit, Price, Sq Ft, Availability, Unit, 194, price, $1,619, square feet, 1,150, availibility, Now, Unit 194, Unit, 105, price, $1,619, square feet, 1,150, availibility, Now, Unit 105, Unit, 245, price, $1,699, square feet, 1,150, availibility, Mar. 16, Unit 245, Show More Results (5), </t>
         </is>
       </c>
     </row>
@@ -4416,40 +4416,40 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Summer Gate</t>
+          <t>Dominion at Mercer Crossing</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/summer-gate-irving-tx/xlw9lem/</t>
+          <t>https://www.apartments.com/dominion-at-mercer-crossing-farmers-branch-tx/6rgqd5v/</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3801 N Belt Line Rd, Irving, TX 75038</t>
+          <t>11771 Mira Lago Blvd, Farmers Branch, TX 75234</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Northwest Dallas</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>1,638</t>
+          <t>2,019</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>974</t>
+          <t>1,295</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>1.681724845995893</v>
+        <v>1.559073359073359</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="J47" t="b">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>2.3</t>
         </is>
       </c>
       <c r="O47" t="b">
@@ -4492,7 +4492,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2, $1,638, 2 beds, 2 baths, 974 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Cable Ready, Security System, Trash Compactor, Storage Units, Fireplace, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Warming Drawer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Dining Room, Walk-In Closets, Window Coverings, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1106, price, $1,638, square feet, 974, availibility, Mar. 23, Unit 1106, </t>
+          <t xml:space="preserve">B3, $2,019 – $2,049, 2 beds, 2 baths, 1,295 sq ft, Tour This Floor Plan, View B3, Floor Plan, View B3 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Satellite TV, Storage Units, Double Vanities, Tub/Shower, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Porch, Deck, Yard, Hardwood Floors, Carpet, Dining Room, Walk-In Closets, Double Pane Windows, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 1243, price, $2,019, square feet, 1,295, availibility, Now, Unit 1243, Unit, 1204, price, $2,049, square feet, 1,295, availibility, Apr. 8, Unit 1204, </t>
         </is>
       </c>
     </row>
@@ -4502,36 +4502,36 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Lexington at Valley Ranch</t>
+          <t>Summer Gate</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/lexington-at-valley-ranch-irving-tx/0sk6mz3/</t>
+          <t>https://www.apartments.com/summer-gate-irving-tx/xlw9lem/</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>202 Santa Fe Trl, Irving, TX 75063</t>
+          <t>3801 N Belt Line Rd, Irving, TX 75038</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Valley Ranch</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>1,929</t>
+          <t>1,638</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>1,135</t>
+          <t>974</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>1.699559471365639</v>
+        <v>1.681724845995893</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -4542,7 +4542,7 @@
         <v>1</v>
       </c>
       <c r="K48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48" t="b">
         <v>1</v>
@@ -4552,7 +4552,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="O48" t="b">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2, $1,929 – $2,812, 2 beds, 2 baths, 1,135 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Satellite TV, Security System, Trash Compactor, Storage Units, Tub/Shower, Fireplace, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Breakfast Nook, Floor Plan Details, Balcony, Patio, Deck, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Family Room, Office, Den, Built-In Bookshelves, Crown Molding, Bay Window, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 3088, price, $1,929, square feet, 1,135, availibility, Mar. 25, Unit 3088, Unit, 2018, price, $1,954, square feet, 1,135, availibility, Mar. 29, Unit 2018, Unit, 3013, price, $1,929, square feet, 1,135, availibility, May 20, Unit 3013, </t>
+          <t xml:space="preserve">B2, $1,638, 2 beds, 2 baths, 974 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Cable Ready, Security System, Trash Compactor, Storage Units, Fireplace, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Warming Drawer, Floor Plan Details, Balcony, Patio, Yard, Hardwood Floors, Carpet, Dining Room, Walk-In Closets, Window Coverings, Large Bedrooms, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1106, price, $1,638, square feet, 974, availibility, Mar. 23, Unit 1106, </t>
         </is>
       </c>
     </row>
@@ -4588,40 +4588,40 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Woodland Hills</t>
+          <t>Lexington at Valley Ranch</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/woodland-hills-irving-tx/26fj6tb/</t>
+          <t>https://www.apartments.com/lexington-at-valley-ranch-irving-tx/0sk6mz3/</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3541 W Northgate Dr, Irving, TX 75062</t>
+          <t>202 Santa Fe Trl, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Valley Ranch</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1,628</t>
+          <t>1,929</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>856</t>
+          <t>1,135</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>1.901869158878505</v>
+        <v>1.699559471365639</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Sycamore</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="J49" t="b">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="O49" t="b">
@@ -4664,7 +4664,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sycamore, $1,628 – $1,916, 2 beds, 2 baths, 856 sq ft, Mar. 17, Tour This Floor Plan, View Sycamore, Photos, View Sycamore, Floor Plan, View Sycamore, Virtual Tours, View Sycamore Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Pantry, Kitchen, Microwave, Oven, Refrigerator, Freezer, Floor Plan Details, Yard, Carpet, Vinyl Flooring, Dining Room, Walk-In Closets, </t>
+          <t xml:space="preserve">B2, $1,929 – $2,812, 2 beds, 2 baths, 1,135 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Satellite TV, Security System, Trash Compactor, Storage Units, Tub/Shower, Fireplace, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Breakfast Nook, Floor Plan Details, Balcony, Patio, Deck, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Family Room, Office, Den, Built-In Bookshelves, Crown Molding, Bay Window, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 3088, price, $1,929, square feet, 1,135, availibility, Mar. 25, Unit 3088, Unit, 2018, price, $1,954, square feet, 1,135, availibility, Mar. 29, Unit 2018, Unit, 3013, price, $1,929, square feet, 1,135, availibility, May 20, Unit 3013, </t>
         </is>
       </c>
     </row>
@@ -4674,17 +4674,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Woodmeade</t>
+          <t>Woodland Hills</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/woodmeade-irving-tx/ckgm3we/</t>
+          <t>https://www.apartments.com/woodland-hills-irving-tx/26fj6tb/</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3801-3929 Block Dr, Irving, TX 75038</t>
+          <t>3541 W Northgate Dr, Irving, TX 75062</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -4694,27 +4694,27 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>1,450</t>
+          <t>1,628</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>952</t>
+          <t>856</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>1.523109243697479</v>
+        <v>1.901869158878505</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>Sycamore</t>
         </is>
       </c>
       <c r="J50" t="b">
         <v>1</v>
       </c>
       <c r="K50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50" t="b">
         <v>1</v>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="O50" t="b">
@@ -4746,11 +4746,11 @@
         <v>1</v>
       </c>
       <c r="U50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $1,450 – $1,467, 2 beds, 2 baths, 952 sq ft, Tour This Floor Plan, View B1, Photos, View B1, Floor Plan, View B1, Virtual Tours, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Ceiling Fans, Cable Ready, Storage Units, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Pantry, Kitchen, Microwave, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Tile Floors, Dining Room, Built-In Bookshelves, Vaulted Ceiling, Views, Walk-In Closets, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 0126, price, $1,450, square feet, 952, availibility, Mar. 20, Unit 0126, </t>
+          <t xml:space="preserve">Sycamore, $1,628 – $1,916, 2 beds, 2 baths, 856 sq ft, Mar. 17, Tour This Floor Plan, View Sycamore, Photos, View Sycamore, Floor Plan, View Sycamore, Virtual Tours, View Sycamore Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Pantry, Kitchen, Microwave, Oven, Refrigerator, Freezer, Floor Plan Details, Yard, Carpet, Vinyl Flooring, Dining Room, Walk-In Closets, </t>
         </is>
       </c>
     </row>
@@ -4760,40 +4760,40 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Portofino at Las Colinas</t>
+          <t>Woodmeade</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/portofino-at-las-colinas-farmers-branch-tx/fs4r0rr/</t>
+          <t>https://www.apartments.com/woodmeade-irving-tx/ckgm3we/</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>11601 Lago Vista W, Farmers Branch, TX 75234</t>
+          <t>3801-3929 Block Dr, Irving, TX 75038</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>1,858</t>
+          <t>1,450</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>1,113</t>
+          <t>952</t>
         </is>
       </c>
       <c r="H51" t="n">
-        <v>1.669362084456424</v>
+        <v>1.523109243697479</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2 BED / 2 BATH</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J51" t="b">
@@ -4810,7 +4810,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="O51" t="b">
@@ -4832,11 +4832,11 @@
         <v>1</v>
       </c>
       <c r="U51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 BED / 2 BATH, $1,858 – $1,893, 2 beds, 2 baths, 1,113 sq ft, $250 deposit, Tour This Floor Plan, View 2 BED / 2 BATH, Floor Plan, View 2 BED / 2 BATH Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Trash Compactor, Double Vanities, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Oven, Range, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Vaulted Ceiling, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 1137, price, $1,883, square feet, 1,113, availibility, Mar. 19, Unit 1137, Unit, 1422, price, $1,893, square feet, 1,113, availibility, Apr. 30, Unit 1422, Unit, 1255, price, $1,858, square feet, 1,113, availibility, May 7, Unit 1255, </t>
+          <t xml:space="preserve">B1, $1,450 – $1,467, 2 beds, 2 baths, 952 sq ft, Tour This Floor Plan, View B1, Photos, View B1, Floor Plan, View B1, Virtual Tours, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Ceiling Fans, Cable Ready, Storage Units, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Pantry, Kitchen, Microwave, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Tile Floors, Dining Room, Built-In Bookshelves, Vaulted Ceiling, Views, Walk-In Closets, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 0126, price, $1,450, square feet, 952, availibility, Mar. 20, Unit 0126, </t>
         </is>
       </c>
     </row>
@@ -4846,47 +4846,47 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Wildwood Creek</t>
+          <t>Portofino at Las Colinas</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/wildwood-creek-grapevine-tx/5j7f2mq/</t>
+          <t>https://www.apartments.com/portofino-at-las-colinas-farmers-branch-tx/fs4r0rr/</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>820 E Dove Loop Rd, Grapevine, TX 76051</t>
+          <t>11601 Lago Vista W, Farmers Branch, TX 75234</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Grapevine</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2,038</t>
+          <t>1,858</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>1,124</t>
+          <t>1,113</t>
         </is>
       </c>
       <c r="H52" t="n">
-        <v>1.813167259786477</v>
+        <v>1.669362084456424</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>The Conservatory - 1124</t>
+          <t>2 BED / 2 BATH</t>
         </is>
       </c>
       <c r="J52" t="b">
         <v>1</v>
       </c>
       <c r="K52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52" t="b">
         <v>1</v>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Conservatory - 1124, $2,038 – $2,221, 2 beds, 2 baths, 1,124 sq ft, Tour This Floor Plan, View The Conservatory - 1124, Floor Plan, View The Conservatory - 1124 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Dining Room, Built-In Bookshelves, Crown Molding, Vaulted Ceiling, Walk-In Closets, 4 Available units, Unit, Price, Sq Ft, Availability, Unit, 0122, price, $2,100, square feet, 1,124, availibility, Now, Unit 0122, Unit, 2223, price, $2,100, square feet, 1,124, availibility, Now, Unit 2223, Unit, 1423, price, $2,052, square feet, 1,124, availibility, May 14, Unit 1423, Show More Results (1), </t>
+          <t xml:space="preserve">2 BED / 2 BATH, $1,858 – $1,893, 2 beds, 2 baths, 1,113 sq ft, $250 deposit, Tour This Floor Plan, View 2 BED / 2 BATH, Floor Plan, View 2 BED / 2 BATH Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Trash Compactor, Double Vanities, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Oven, Range, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Vaulted Ceiling, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 1137, price, $1,883, square feet, 1,113, availibility, Mar. 19, Unit 1137, Unit, 1422, price, $1,893, square feet, 1,113, availibility, Apr. 30, Unit 1422, Unit, 1255, price, $1,858, square feet, 1,113, availibility, May 7, Unit 1255, </t>
         </is>
       </c>
     </row>
@@ -4932,47 +4932,47 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Mercer Crossing Apartments</t>
+          <t>Wildwood Creek</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/mercer-crossing-apartments-farmers-branch-tx/ry5dl00/</t>
+          <t>https://www.apartments.com/wildwood-creek-grapevine-tx/5j7f2mq/</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>11700 Luna Rd, Farmers Branch, TX 75234</t>
+          <t>820 E Dove Loop Rd, Grapevine, TX 76051</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Koreatown/Gribble</t>
+          <t>Grapevine</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>1,909</t>
+          <t>2,038</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>1,098</t>
+          <t>1,124</t>
         </is>
       </c>
       <c r="H53" t="n">
-        <v>1.738615664845173</v>
+        <v>1.813167259786477</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>The Conservatory - 1124</t>
         </is>
       </c>
       <c r="J53" t="b">
         <v>1</v>
       </c>
       <c r="K53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53" t="b">
         <v>1</v>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="O53" t="b">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $1,909 – $1,914, 2 beds, 2 baths, 1,098 sq ft, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Handrails, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Porch, Yard, Lawn, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Office, Built-In Bookshelves, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 06301, price, $1,909, square feet, 1,098, availibility, Now, Unit 06301, Unit, 05101, price, $1,914, square feet, 1,098, availibility, May 15, Unit 05101, </t>
+          <t xml:space="preserve">The Conservatory - 1124, $2,038 – $2,221, 2 beds, 2 baths, 1,124 sq ft, Tour This Floor Plan, View The Conservatory - 1124, Floor Plan, View The Conservatory - 1124 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Ceiling Fans, Cable Ready, Storage Units, Double Vanities, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Dining Room, Built-In Bookshelves, Crown Molding, Vaulted Ceiling, Walk-In Closets, 4 Available units, Unit, Price, Sq Ft, Availability, Unit, 0122, price, $2,100, square feet, 1,124, availibility, Now, Unit 0122, Unit, 2223, price, $2,100, square feet, 1,124, availibility, Now, Unit 2223, Unit, 1423, price, $2,052, square feet, 1,124, availibility, May 14, Unit 1423, Show More Results (1), </t>
         </is>
       </c>
     </row>
@@ -5018,40 +5018,40 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>AMLI at Escena</t>
+          <t>Mercer Crossing Apartments</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/amli-at-escena-irving-tx/8wxlrr2/</t>
+          <t>https://www.apartments.com/mercer-crossing-apartments-farmers-branch-tx/ry5dl00/</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>6401 Escena Blvd, Irving, TX 75039</t>
+          <t>11700 Luna Rd, Farmers Branch, TX 75234</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Las Colinas</t>
+          <t>Koreatown/Gribble</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2,073</t>
+          <t>1,909</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>1,105</t>
+          <t>1,098</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>1.876018099547511</v>
+        <v>1.738615664845173</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>C4</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J54" t="b">
@@ -5068,7 +5068,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="O54" t="b">
@@ -5094,7 +5094,7 @@
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t xml:space="preserve">C4, $2,073 – $2,883, 2 beds, 2 baths, 1,105 sq ft, $500 deposit, Available Now, Tour This Floor Plan, View C4, Floor Plan, View C4 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Lawn, Garden, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Den, Walk-In Closets, Furnished, Window Coverings, Large Bedrooms, </t>
+          <t xml:space="preserve">B1, $1,909 – $1,914, 2 beds, 2 baths, 1,098 sq ft, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Trash Compactor, Storage Units, Double Vanities, Tub/Shower, Handrails, Sprinkler System, Framed Mirrors, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Eat-in Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Porch, Yard, Lawn, Hardwood Floors, Carpet, Tile Floors, Vinyl Flooring, Dining Room, Office, Built-In Bookshelves, Views, Walk-In Closets, Linen Closet, Double Pane Windows, Window Coverings, Large Bedrooms, 2 Available units, Unit, Price, Sq Ft, Availability, Unit, 06301, price, $1,909, square feet, 1,098, availibility, Now, Unit 06301, Unit, 05101, price, $1,914, square feet, 1,098, availibility, May 15, Unit 05101, </t>
         </is>
       </c>
     </row>
@@ -5190,17 +5190,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Jefferson Creek</t>
+          <t>AMLI at Escena</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/jefferson-creek-irving-tx/vr37bee/</t>
+          <t>https://www.apartments.com/amli-at-escena-irving-tx/8wxlrr2/</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>800 W Royal Ln, Irving, TX 75039</t>
+          <t>6401 Escena Blvd, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -5210,20 +5210,20 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>1,817</t>
+          <t>2,073</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>1,186</t>
+          <t>1,105</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>1.53204047217538</v>
+        <v>1.876018099547511</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>C4</t>
         </is>
       </c>
       <c r="J56" t="b">
@@ -5240,7 +5240,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="O56" t="b">
@@ -5266,7 +5266,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t xml:space="preserve">B2, $1,817 – $1,833, 2 beds, 2 baths, 1,186 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Tub/Shower, Fireplace, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Office, Den, Vaulted Ceiling, Walk-In Closets, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 382, price, $1,817, square feet, 1,186, availibility, Now, Unit 382, </t>
+          <t xml:space="preserve">C4, $2,073 – $2,883, 2 beds, 2 baths, 1,105 sq ft, $500 deposit, Available Now, Tour This Floor Plan, View C4, Floor Plan, View C4 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Tub/Shower, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Stainless Steel Appliances, Pantry, Island Kitchen, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Yard, Lawn, Garden, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Family Room, Office, Den, Walk-In Closets, Furnished, Window Coverings, Large Bedrooms, </t>
         </is>
       </c>
     </row>
@@ -5276,17 +5276,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Jefferson Place</t>
+          <t>Jefferson Creek</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/jefferson-place-irving-tx/2kzf7sc/</t>
+          <t>https://www.apartments.com/jefferson-creek-irving-tx/vr37bee/</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>6306 N MacArthur Blvd, Irving, TX 75039</t>
+          <t>800 W Royal Ln, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -5296,20 +5296,20 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>1,649</t>
+          <t>1,817</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>921</t>
+          <t>1,186</t>
         </is>
       </c>
       <c r="H57" t="n">
-        <v>1.790445168295331</v>
+        <v>1.53204047217538</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="J57" t="b">
@@ -5326,7 +5326,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="O57" t="b">
@@ -5352,7 +5352,7 @@
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $1,649 – $1,704, 2 beds, 2 baths, 921 sq ft, Mar. 16, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Tub/Shower, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Office, Vaulted Ceiling, Walk-In Closets, Window Coverings, </t>
+          <t xml:space="preserve">B2, $1,817 – $1,833, 2 beds, 2 baths, 1,186 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Tub/Shower, Fireplace, Sprinkler System, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Office, Den, Vaulted Ceiling, Walk-In Closets, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 382, price, $1,817, square feet, 1,186, availibility, Now, Unit 382, </t>
         </is>
       </c>
     </row>
@@ -5362,17 +5362,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Arbors of Las Colinas</t>
+          <t>Jefferson Place</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/arbors-of-las-colinas-irving-tx/3gxz0dg/</t>
+          <t>https://www.apartments.com/jefferson-place-irving-tx/2kzf7sc/</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1000 San Jacinto Dr, Irving, TX 75063</t>
+          <t>6306 N MacArthur Blvd, Irving, TX 75039</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -5382,20 +5382,20 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>1,693</t>
+          <t>1,649</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>1,139</t>
+          <t>921</t>
         </is>
       </c>
       <c r="H58" t="n">
-        <v>1.486391571553995</v>
+        <v>1.790445168295331</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>Willow</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J58" t="b">
@@ -5412,7 +5412,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="O58" t="b">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Willow, $1,693, 2 beds, 2 baths, 1,139 sq ft, Tour This Floor Plan, View Willow, Floor Plan, View Willow Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Attic, Vaulted Ceiling, Walk-In Closets, Linen Closet, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1221, price, $1,693, square feet, 1,139, availibility, Now, Unit 1221, </t>
+          <t xml:space="preserve">B1, $1,649 – $1,704, 2 beds, 2 baths, 921 sq ft, Mar. 16, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Storage Units, Tub/Shower, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Office, Vaulted Ceiling, Walk-In Closets, Window Coverings, </t>
         </is>
       </c>
     </row>
@@ -5448,17 +5448,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>MARFA Apartments</t>
+          <t>Arbors of Las Colinas</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/marfa-apartments-irving-tx/e143xsn/</t>
+          <t>https://www.apartments.com/arbors-of-las-colinas-irving-tx/3gxz0dg/</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2727 W Walnut Hill Ln, Irving, TX 75038</t>
+          <t>1000 San Jacinto Dr, Irving, TX 75063</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -5468,27 +5468,27 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>1,329</t>
+          <t>1,693</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>819</t>
+          <t>1,139</t>
         </is>
       </c>
       <c r="H59" t="n">
-        <v>1.622710622710623</v>
+        <v>1.486391571553995</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>Willow</t>
         </is>
       </c>
       <c r="J59" t="b">
         <v>1</v>
       </c>
       <c r="K59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L59" t="b">
         <v>1</v>
@@ -5498,7 +5498,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="O59" t="b">
@@ -5524,7 +5524,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t xml:space="preserve">B1, $1,329, 2 beds, 2 baths, 819 sq ft, Available Now, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Kitchen, Microwave, Oven, Refrigerator, Freezer, Instant Hot Water, Floor Plan Details, Balcony, Patio, Hardwood Floors, Skylight, Walk-In Closets, </t>
+          <t xml:space="preserve">Willow, $1,693, 2 beds, 2 baths, 1,139 sq ft, Tour This Floor Plan, View Willow, Floor Plan, View Willow Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Tub/Shower, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Attic, Vaulted Ceiling, Walk-In Closets, Linen Closet, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1221, price, $1,693, square feet, 1,139, availibility, Now, Unit 1221, </t>
         </is>
       </c>
     </row>
@@ -5534,40 +5534,40 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Summerwood Apartments</t>
+          <t>MARFA Apartments</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/summerwood-apartments-irving-tx/vpjhb8f/</t>
+          <t>https://www.apartments.com/marfa-apartments-irving-tx/e143xsn/</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>4132 N Belt Line Rd, Irving, TX 75038</t>
+          <t>2727 W Walnut Hill Ln, Irving, TX 75038</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Las Colinas</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>1,200</t>
+          <t>1,329</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>1,030</t>
+          <t>819</t>
         </is>
       </c>
       <c r="H60" t="n">
-        <v>1.16504854368932</v>
+        <v>1.622710622710623</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>B-1</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="J60" t="b">
@@ -5584,7 +5584,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="O60" t="b">
@@ -5606,11 +5606,11 @@
         <v>1</v>
       </c>
       <c r="U60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t xml:space="preserve">B-1, $1,200 – $1,350, 2 beds, 2 baths, 1,030 sq ft, 6 – 12 Month Lease, Mar. 28, Tour This Floor Plan, View B-1, Floor Plan, View B-1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Tub/Shower, Fireplace, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Granite Countertops, Pantry, Kitchen, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Carpet, Vinyl Flooring, Dining Room, Den, Views, Walk-In Closets, Linen Closet, Window Coverings, </t>
+          <t xml:space="preserve">B1, $1,329, 2 beds, 2 baths, 819 sq ft, Available Now, Tour This Floor Plan, View B1, Floor Plan, View B1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Fireplace, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Kitchen, Microwave, Oven, Refrigerator, Freezer, Instant Hot Water, Floor Plan Details, Balcony, Patio, Hardwood Floors, Skylight, Walk-In Closets, </t>
         </is>
       </c>
     </row>
@@ -5620,40 +5620,40 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Cobblestone Village</t>
+          <t>Summerwood Apartments</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/cobblestone-village-grapevine-tx/vvym7kg/</t>
+          <t>https://www.apartments.com/summerwood-apartments-irving-tx/vpjhb8f/</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>951 Turner Rd, Grapevine, TX 76051</t>
+          <t>4132 N Belt Line Rd, Irving, TX 75038</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Grapevine</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>1,380</t>
+          <t>1,200</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>1,042</t>
+          <t>1,030</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>1.324376199616123</v>
+        <v>1.16504854368932</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Gneiss</t>
+          <t>B-1</t>
         </is>
       </c>
       <c r="J61" t="b">
@@ -5670,7 +5670,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="O61" t="b">
@@ -5692,11 +5692,11 @@
         <v>1</v>
       </c>
       <c r="U61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gneiss, $1,380, 2 beds, 2 baths, 1,042 sq ft, $300 deposit, Tour This Floor Plan, View Gneiss, Photos, View Gneiss, Floor Plan, View Gneiss Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Storage Units, Tub/Shower, Fireplace, Framed Mirrors, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Carpet, Vinyl Flooring, Dining Room, Walk-In Closets, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 525, price, $1,380, square feet, 1,042, availibility, May 18, Unit 525, </t>
+          <t xml:space="preserve">B-1, $1,200 – $1,350, 2 beds, 2 baths, 1,030 sq ft, 6 – 12 Month Lease, Mar. 28, Tour This Floor Plan, View B-1, Floor Plan, View B-1 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Cable Ready, Security System, Tub/Shower, Fireplace, Sprinkler System, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Granite Countertops, Pantry, Kitchen, Oven, Range, Refrigerator, Floor Plan Details, Balcony, Carpet, Vinyl Flooring, Dining Room, Den, Views, Walk-In Closets, Linen Closet, Window Coverings, </t>
         </is>
       </c>
     </row>
@@ -5706,40 +5706,40 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sevilla Condos</t>
+          <t>Cobblestone Village</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://www.apartments.com/sevilla-condos-carrollton-tx/qnwem8z/</t>
+          <t>https://www.apartments.com/cobblestone-village-grapevine-tx/vvym7kg/</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1455 N Perry Rd, Carrollton, TX 75006</t>
+          <t>951 Turner Rd, Grapevine, TX 76051</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Original Town</t>
+          <t>Grapevine</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>1,410</t>
+          <t>1,380</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>992</t>
+          <t>1,042</t>
         </is>
       </c>
       <c r="H62" t="n">
-        <v>1.421370967741935</v>
+        <v>1.324376199616123</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>2 Bed 2 Bath w/study - upgraded</t>
+          <t>Gneiss</t>
         </is>
       </c>
       <c r="J62" t="b">
@@ -5756,7 +5756,7 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="O62" t="b">
@@ -5778,11 +5778,11 @@
         <v>1</v>
       </c>
       <c r="U62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 Bed 2 Bath w/study - upgraded, $1,410, 2 beds, 2 baths, 992 sq ft, Tour This Floor Plan, View 2 Bed 2 Bath w/study - upgraded, Floor Plan, View 2 Bed 2 Bath w/study - upgraded Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Tub/Shower, Fireplace, Handrails, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Den, Walk-In Closets, Linen Closet, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1206, price, $1,410, square feet, 992, availibility, Apr. 26, Unit 1206, </t>
+          <t xml:space="preserve">Gneiss, $1,380, 2 beds, 2 baths, 1,042 sq ft, $300 deposit, Tour This Floor Plan, View Gneiss, Photos, View Gneiss, Floor Plan, View Gneiss Floor Plan Details, Show Floor Plan Details, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 525, price, $1,380, square feet, 1,042, availibility, May 18, Unit 525, </t>
         </is>
       </c>
     </row>
@@ -5792,81 +5792,167 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>Sevilla Condos</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://www.apartments.com/sevilla-condos-carrollton-tx/qnwem8z/</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>1455 N Perry Rd, Carrollton, TX 75006</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Original Town</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>1,410</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>992</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>1.421370967741935</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2 Bed 2 Bath w/study - upgraded</t>
+        </is>
+      </c>
+      <c r="J63" t="b">
+        <v>1</v>
+      </c>
+      <c r="K63" t="b">
+        <v>0</v>
+      </c>
+      <c r="L63" t="b">
+        <v>1</v>
+      </c>
+      <c r="M63" t="b">
+        <v>1</v>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>2.2</t>
+        </is>
+      </c>
+      <c r="O63" t="b">
+        <v>1</v>
+      </c>
+      <c r="P63" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q63" t="b">
+        <v>1</v>
+      </c>
+      <c r="R63" t="b">
+        <v>1</v>
+      </c>
+      <c r="S63" t="b">
+        <v>1</v>
+      </c>
+      <c r="T63" t="b">
+        <v>1</v>
+      </c>
+      <c r="U63" t="b">
+        <v>0</v>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 Bed 2 Bath w/study - upgraded, $1,410, 2 beds, 2 baths, 992 sq ft, Tour This Floor Plan, View 2 Bed 2 Bath w/study - upgraded, Floor Plan, View 2 Bed 2 Bath w/study - upgraded Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Ceiling Fans, Smoke Free, Cable Ready, Tub/Shower, Fireplace, Handrails, Kitchen Features &amp; Appliances, Dishwasher, Disposal, Stainless Steel Appliances, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Vinyl Flooring, Dining Room, Office, Den, Walk-In Closets, Linen Closet, Window Coverings, 1 Available unit, Unit, Price, Sq Ft, Availability, Unit, 1206, price, $1,410, square feet, 992, availibility, Apr. 26, Unit 1206, </t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
           <t>Hidden Ridge On The Canal</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C64" t="inlineStr">
         <is>
           <t>https://www.apartments.com/hidden-ridge-on-the-canal-irving-tx/9ezmbe4/</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>1290 Hidden Rd, Irving, TX 75038</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>Las Colinas</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="F64" t="inlineStr">
         <is>
           <t>1,355</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
+      <c r="G64" t="inlineStr">
         <is>
           <t>1,088</t>
         </is>
       </c>
-      <c r="H63" t="n">
+      <c r="H64" t="n">
         <v>1.245404411764706</v>
       </c>
-      <c r="I63" t="inlineStr">
+      <c r="I64" t="inlineStr">
         <is>
           <t>B2</t>
         </is>
       </c>
-      <c r="J63" t="b">
-        <v>1</v>
-      </c>
-      <c r="K63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L63" t="b">
-        <v>1</v>
-      </c>
-      <c r="M63" t="b">
-        <v>1</v>
-      </c>
-      <c r="N63" t="inlineStr">
+      <c r="J64" t="b">
+        <v>1</v>
+      </c>
+      <c r="K64" t="b">
+        <v>1</v>
+      </c>
+      <c r="L64" t="b">
+        <v>1</v>
+      </c>
+      <c r="M64" t="b">
+        <v>1</v>
+      </c>
+      <c r="N64" t="inlineStr">
         <is>
           <t>2.0</t>
         </is>
       </c>
-      <c r="O63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P63" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q63" t="b">
-        <v>1</v>
-      </c>
-      <c r="R63" t="b">
-        <v>1</v>
-      </c>
-      <c r="S63" t="b">
-        <v>1</v>
-      </c>
-      <c r="T63" t="b">
-        <v>1</v>
-      </c>
-      <c r="U63" t="b">
-        <v>1</v>
-      </c>
-      <c r="V63" t="inlineStr">
+      <c r="O64" t="b">
+        <v>1</v>
+      </c>
+      <c r="P64" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q64" t="b">
+        <v>1</v>
+      </c>
+      <c r="R64" t="b">
+        <v>1</v>
+      </c>
+      <c r="S64" t="b">
+        <v>1</v>
+      </c>
+      <c r="T64" t="b">
+        <v>1</v>
+      </c>
+      <c r="U64" t="b">
+        <v>1</v>
+      </c>
+      <c r="V64" t="inlineStr">
         <is>
           <t xml:space="preserve">B2, $1,355 – $1,495, 2 beds, 2 baths, 1,088 sq ft, Tour This Floor Plan, View B2, Floor Plan, View B2 Floor Plan Details, Hide Floor Plan Details, Highlights, High Speed Internet Access, Wi-Fi, In Unit Washer &amp; Dryer, Washer/Dryer Hookup, Air Conditioning, Heating, Cable Ready, Security System, Storage Units, Tub/Shower, Fireplace, Wheelchair Accessible (Rooms), Kitchen Features &amp; Appliances, Dishwasher, Disposal, Ice Maker, Granite Countertops, Pantry, Kitchen, Microwave, Oven, Range, Refrigerator, Freezer, Floor Plan Details, Balcony, Patio, Hardwood Floors, Carpet, Dining Room, Den, Views, Walk-In Closets, Window Coverings, Large Bedrooms, 3 Available units, Unit, Price, Sq Ft, Availability, Unit, 3130, price, $1,355, square feet, 1,088, availibility, Apr. 23, Unit 3130, Unit, 2107, price, $1,395, square feet, 1,088, availibility, Apr. 23, Unit 2107, Unit, 3068, price, $1,475, square feet, 1,088, availibility, Apr. 23, Unit 3068, </t>
         </is>

</xml_diff>